<commit_message>
post refurb oxide cleaning didn't happen on primary side - maybe fixed
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -431,1716 +431,1716 @@
         <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.03045833333333333</v>
+        <v>0.030375</v>
       </c>
       <c r="C2">
-        <v>0.05015783118506079</v>
+        <v>0.04758436596421234</v>
       </c>
       <c r="D2">
-        <v>261.8440597705786</v>
+        <v>261.8437209902542</v>
       </c>
       <c r="E2">
-        <v>0.009791998717485406</v>
+        <v>0.00979046879271926</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>30444</v>
+        <v>30444.41666666667</v>
       </c>
       <c r="B3">
-        <v>0.03091666666666667</v>
+        <v>0.03075</v>
       </c>
       <c r="C3">
-        <v>0.07175498635729127</v>
+        <v>0.06781343148509222</v>
       </c>
       <c r="D3">
-        <v>261.8942176017637</v>
+        <v>261.8913053562184</v>
       </c>
       <c r="E3">
-        <v>0.01001851042023139</v>
+        <v>0.0100053587810617</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>30475</v>
+        <v>30474.83333333333</v>
       </c>
       <c r="B4">
-        <v>0.031375</v>
+        <v>0.031125</v>
       </c>
       <c r="C4">
-        <v>0.07587502821365888</v>
+        <v>0.07226058654373446</v>
       </c>
       <c r="D4">
-        <v>261.965972588121</v>
+        <v>261.9591187877035</v>
       </c>
       <c r="E4">
-        <v>0.0103425544180736</v>
+        <v>0.0103116028006258</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>30505</v>
+        <v>30505.25</v>
       </c>
       <c r="B5">
-        <v>0.03183333333333333</v>
+        <v>0.0315</v>
       </c>
       <c r="C5">
-        <v>0.07644353032344497</v>
+        <v>0.07304537307322789</v>
       </c>
       <c r="D5">
-        <v>262.0418476163346</v>
+        <v>262.0313793742472</v>
       </c>
       <c r="E5">
-        <v>0.01068520443763202</v>
+        <v>0.01063793007819598</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>30536</v>
+        <v>30535.66666666667</v>
       </c>
       <c r="B6">
-        <v>0.03229166666666666</v>
+        <v>0.031875</v>
       </c>
       <c r="C6">
-        <v>0.07687629107840621</v>
+        <v>0.07245088788226894</v>
       </c>
       <c r="D6">
-        <v>262.1182911466581</v>
+        <v>262.1044247473204</v>
       </c>
       <c r="E6">
-        <v>0.01103042180067127</v>
+        <v>0.01096780143510284</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2">
-        <v>30567</v>
+        <v>30566.08333333333</v>
       </c>
       <c r="B7">
-        <v>0.03274999999999999</v>
+        <v>0.03225</v>
       </c>
       <c r="C7">
-        <v>0.0786876710907336</v>
+        <v>0.07323362209717743</v>
       </c>
       <c r="D7">
-        <v>262.1951674377365</v>
+        <v>262.1768756352027</v>
       </c>
       <c r="E7">
-        <v>0.01137759350210926</v>
+        <v>0.01129498810948523</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2">
-        <v>30597</v>
+        <v>30596.5</v>
       </c>
       <c r="B8">
-        <v>0.03320833333333333</v>
+        <v>0.032625</v>
       </c>
       <c r="C8">
-        <v>0.07752973292622301</v>
+        <v>0.07307704440938778</v>
       </c>
       <c r="D8">
-        <v>262.2738551088272</v>
+        <v>262.2501092572999</v>
       </c>
       <c r="E8">
-        <v>0.01173294535729834</v>
+        <v>0.01162570959499505</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
-        <v>30628</v>
+        <v>30626.91666666667</v>
       </c>
       <c r="B9">
-        <v>0.03366666666666666</v>
+        <v>0.033</v>
       </c>
       <c r="C9">
-        <v>0.07500930541732487</v>
+        <v>0.07181463969470769</v>
       </c>
       <c r="D9">
-        <v>262.3513848417534</v>
+        <v>262.3231863017093</v>
       </c>
       <c r="E9">
-        <v>0.01208306798827416</v>
+        <v>0.01195572397898507</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2">
-        <v>30658</v>
+        <v>30657.33333333333</v>
       </c>
       <c r="B10">
-        <v>0.03412499999999999</v>
+        <v>0.033375</v>
       </c>
       <c r="C10">
-        <v>0.0760707614228977</v>
+        <v>0.07265737143029583</v>
       </c>
       <c r="D10">
-        <v>262.4263941471708</v>
+        <v>262.395000941404</v>
       </c>
       <c r="E10">
-        <v>0.01242180842202993</v>
+        <v>0.01228003737003494</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2">
-        <v>30689</v>
+        <v>30687.75</v>
       </c>
       <c r="B11">
-        <v>0.03458333333333332</v>
+        <v>0.03375</v>
       </c>
       <c r="C11">
-        <v>0.07810538954390722</v>
+        <v>0.07419024397836438</v>
       </c>
       <c r="D11">
-        <v>262.5024649085937</v>
+        <v>262.4676583128343</v>
       </c>
       <c r="E11">
-        <v>0.01276534236861353</v>
+        <v>0.01260815651974448</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2">
-        <v>30720</v>
+        <v>30718.16666666667</v>
       </c>
       <c r="B12">
-        <v>0.03504166666666665</v>
+        <v>0.034125</v>
       </c>
       <c r="C12">
-        <v>0.07598961311055064</v>
+        <v>0.07330373530544421</v>
       </c>
       <c r="D12">
-        <v>262.5805702981376</v>
+        <v>262.5418485568126</v>
       </c>
       <c r="E12">
-        <v>0.01311806465267608</v>
+        <v>0.0129431980893983</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2">
-        <v>30749</v>
+        <v>30748.58333333333</v>
       </c>
       <c r="B13">
-        <v>0.03549999999999998</v>
+        <v>0.0345</v>
       </c>
       <c r="C13">
-        <v>0.0497854511247624</v>
+        <v>0.07030531528232586</v>
       </c>
       <c r="D13">
-        <v>262.6565599112481</v>
+        <v>262.6151522921181</v>
       </c>
       <c r="E13">
-        <v>0.01346123213520086</v>
+        <v>0.01327423620467113</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2">
-        <v>30841</v>
+        <v>30839.83333333333</v>
       </c>
       <c r="B14">
-        <v>0.03595833333333331</v>
+        <v>0.034875</v>
       </c>
       <c r="C14">
-        <v>0.5320105142091052</v>
+        <v>0.5314410271482757</v>
       </c>
       <c r="D14">
-        <v>262.162348121081</v>
+        <v>262.169885506295</v>
       </c>
       <c r="E14">
-        <v>0.01122938216356143</v>
+        <v>0.01126342083546484</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2">
-        <v>30871</v>
+        <v>30870.25</v>
       </c>
       <c r="B15">
-        <v>0.03641666666666665</v>
+        <v>0.03525</v>
       </c>
       <c r="C15">
-        <v>0.1710824395654527</v>
+        <v>0.1662611293193095</v>
       </c>
       <c r="D15">
-        <v>262.6943586352901</v>
+        <v>262.7013265334433</v>
       </c>
       <c r="E15">
-        <v>0.01363193037198824</v>
+        <v>0.01366339725239266</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2">
-        <v>30902</v>
+        <v>30900.66666666667</v>
       </c>
       <c r="B16">
-        <v>0.03687499999999998</v>
+        <v>0.035625</v>
       </c>
       <c r="C16">
-        <v>0.09711162298992804</v>
+        <v>0.09313466017795236</v>
       </c>
       <c r="D16">
-        <v>262.8654410748555</v>
+        <v>262.8675876627626</v>
       </c>
       <c r="E16">
-        <v>0.01440453504368783</v>
+        <v>0.0144142289891882</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <v>30933</v>
+        <v>30931.08333333333</v>
       </c>
       <c r="B17">
-        <v>0.03733333333333331</v>
+        <v>0.036</v>
       </c>
       <c r="C17">
-        <v>0.08268783117375733</v>
+        <v>0.07821425621500566</v>
       </c>
       <c r="D17">
-        <v>262.9625526978455</v>
+        <v>262.9607223229406</v>
       </c>
       <c r="E17">
-        <v>0.01484308907523498</v>
+        <v>0.01483482314095161</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2">
-        <v>30963</v>
+        <v>30961.5</v>
       </c>
       <c r="B18">
-        <v>0.03779166666666664</v>
+        <v>0.036375</v>
       </c>
       <c r="C18">
-        <v>0.08039929953190494</v>
+        <v>0.07516570001030232</v>
       </c>
       <c r="D18">
-        <v>263.0452405290192</v>
+        <v>263.0389365791556</v>
       </c>
       <c r="E18">
-        <v>0.01521650556859224</v>
+        <v>0.01518803706459391</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2">
-        <v>30994</v>
+        <v>30991.91666666667</v>
       </c>
       <c r="B19">
-        <v>0.03824999999999997</v>
+        <v>0.03675</v>
       </c>
       <c r="C19">
-        <v>0.07845547395675112</v>
+        <v>0.07374368110288287</v>
       </c>
       <c r="D19">
-        <v>263.1256398285511</v>
+        <v>263.1141022791659</v>
       </c>
       <c r="E19">
-        <v>0.01557958710155099</v>
+        <v>0.01552748377301725</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2">
-        <v>31024</v>
+        <v>31022.33333333333</v>
       </c>
       <c r="B20">
-        <v>0.0387083333333333</v>
+        <v>0.03712500000000001</v>
       </c>
       <c r="C20">
-        <v>0.07706258736038762</v>
+        <v>0.07400753883848665</v>
       </c>
       <c r="D20">
-        <v>263.2040953025079</v>
+        <v>263.1878459602688</v>
       </c>
       <c r="E20">
-        <v>0.01593389035940338</v>
+        <v>0.01586050867418848</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2">
-        <v>31055</v>
+        <v>31052.75</v>
       </c>
       <c r="B21">
-        <v>0.03916666666666663</v>
+        <v>0.03750000000000001</v>
       </c>
       <c r="C21">
-        <v>0.07852569943338494</v>
+        <v>0.07530938131333187</v>
       </c>
       <c r="D21">
-        <v>263.2811578898683</v>
+        <v>263.2618534991072</v>
       </c>
       <c r="E21">
-        <v>0.01628190337090305</v>
+        <v>0.01619472515130231</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2">
-        <v>31086</v>
+        <v>31083.16666666667</v>
       </c>
       <c r="B22">
-        <v>0.03962499999999997</v>
+        <v>0.03787500000000001</v>
       </c>
       <c r="C22">
-        <v>0.08046678196285484</v>
+        <v>0.07400012180619342</v>
       </c>
       <c r="D22">
-        <v>263.3596835893017</v>
+        <v>263.3371628804206</v>
       </c>
       <c r="E22">
-        <v>0.01663652376551992</v>
+        <v>0.0165348207214455</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2">
-        <v>31114</v>
+        <v>31113.58333333333</v>
       </c>
       <c r="B23">
-        <v>0.0400833333333333</v>
+        <v>0.03825000000000001</v>
       </c>
       <c r="C23">
-        <v>0.07862686056421353</v>
+        <v>0.07431215058636553</v>
       </c>
       <c r="D23">
-        <v>263.4401503712645</v>
+        <v>263.4111630022268</v>
       </c>
       <c r="E23">
-        <v>0.01699991004770667</v>
+        <v>0.01686900370339847</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2">
-        <v>31145</v>
+        <v>31144</v>
       </c>
       <c r="B24">
-        <v>0.04054166666666663</v>
+        <v>0.03862500000000001</v>
       </c>
       <c r="C24">
-        <v>0.07927311346793431</v>
+        <v>0.0758329166249041</v>
       </c>
       <c r="D24">
-        <v>263.5187772318287</v>
+        <v>263.4854751528131</v>
       </c>
       <c r="E24">
-        <v>0.01735498728384661</v>
+        <v>0.01720459580071081</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2">
-        <v>31175</v>
+        <v>31174.41666666667</v>
       </c>
       <c r="B25">
-        <v>0.04099999999999996</v>
+        <v>0.03900000000000001</v>
       </c>
       <c r="C25">
-        <v>0.07814768655055104</v>
+        <v>0.07581492180202076</v>
       </c>
       <c r="D25">
-        <v>263.5980503452967</v>
+        <v>263.561308069438</v>
       </c>
       <c r="E25">
-        <v>0.01771298298440515</v>
+        <v>0.01754705564522689</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2">
-        <v>31206</v>
+        <v>31204.83333333333</v>
       </c>
       <c r="B26">
-        <v>0.04145833333333329</v>
+        <v>0.03937500000000001</v>
       </c>
       <c r="C26">
-        <v>0.07929311571479047</v>
+        <v>0.07664450655192923</v>
       </c>
       <c r="D26">
-        <v>263.6761980318472</v>
+        <v>263.6371229912401</v>
       </c>
       <c r="E26">
-        <v>0.0180658962808535</v>
+        <v>0.01788943422550406</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2">
-        <v>31236</v>
+        <v>31235.25</v>
       </c>
       <c r="B27">
-        <v>0.04191666666666662</v>
+        <v>0.03975000000000001</v>
       </c>
       <c r="C27">
-        <v>0.07996896597649084</v>
+        <v>0.07653373826997267</v>
       </c>
       <c r="D27">
-        <v>263.755491147562</v>
+        <v>263.713767497792</v>
       </c>
       <c r="E27">
-        <v>0.01842398231113503</v>
+        <v>0.01823555919293217</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2">
-        <v>31267</v>
+        <v>31265.66666666667</v>
       </c>
       <c r="B28">
-        <v>0.04237499999999995</v>
+        <v>0.04012500000000001</v>
       </c>
       <c r="C28">
-        <v>0.07959220181658111</v>
+        <v>0.07756660131553872</v>
       </c>
       <c r="D28">
-        <v>263.8354601135385</v>
+        <v>263.790301236062</v>
       </c>
       <c r="E28">
-        <v>0.01878512046687658</v>
+        <v>0.01858118393314645</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2">
-        <v>31298</v>
+        <v>31296.08333333333</v>
       </c>
       <c r="B29">
-        <v>0.04283333333333329</v>
+        <v>0.04050000000000001</v>
       </c>
       <c r="C29">
-        <v>0.08121864742986418</v>
+        <v>0.07738581269904898</v>
       </c>
       <c r="D29">
-        <v>263.9150523153551</v>
+        <v>263.8678678373775</v>
       </c>
       <c r="E29">
-        <v>0.0191445571636559</v>
+        <v>0.01893147306098718</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2">
-        <v>31328</v>
+        <v>31326.5</v>
       </c>
       <c r="B30">
-        <v>0.04329166666666662</v>
+        <v>0.04087500000000001</v>
       </c>
       <c r="C30">
-        <v>0.08416924116045266</v>
+        <v>0.07996712998692601</v>
       </c>
       <c r="D30">
-        <v>263.9962709627849</v>
+        <v>263.9452536500766</v>
       </c>
       <c r="E30">
-        <v>0.0195113388543589</v>
+        <v>0.01928094575126681</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2">
-        <v>31359</v>
+        <v>31356.91666666667</v>
       </c>
       <c r="B31">
-        <v>0.04374999999999995</v>
+        <v>0.04125000000000001</v>
       </c>
       <c r="C31">
-        <v>0.08274851209830558</v>
+        <v>0.07662654878697595</v>
       </c>
       <c r="D31">
-        <v>264.0804402039454</v>
+        <v>264.0252207800635</v>
       </c>
       <c r="E31">
-        <v>0.01989144536382391</v>
+        <v>0.01964207561571835</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2">
-        <v>31389</v>
+        <v>31387.33333333333</v>
       </c>
       <c r="B32">
-        <v>0.04420833333333328</v>
+        <v>0.04162500000000001</v>
       </c>
       <c r="C32">
-        <v>0.08244254102658033</v>
+        <v>0.07727246314004788</v>
       </c>
       <c r="D32">
-        <v>264.1631887160437</v>
+        <v>264.1018473288505</v>
       </c>
       <c r="E32">
-        <v>0.02026513589095061</v>
+        <v>0.0199881194862605</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2">
-        <v>31420</v>
+        <v>31417.75</v>
       </c>
       <c r="B33">
-        <v>0.04466666666666661</v>
+        <v>0.04200000000000001</v>
       </c>
       <c r="C33">
-        <v>0.08238614409071943</v>
+        <v>0.07661235168870917</v>
       </c>
       <c r="D33">
-        <v>264.2456312570703</v>
+        <v>264.1791197919905</v>
       </c>
       <c r="E33">
-        <v>0.02063744465920116</v>
+        <v>0.02033708029233377</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2">
-        <v>31451</v>
+        <v>31448.16666666667</v>
       </c>
       <c r="B34">
-        <v>0.04512499999999994</v>
+        <v>0.04237500000000001</v>
       </c>
       <c r="C34">
-        <v>0.08204121668291009</v>
+        <v>0.07704546243792265</v>
       </c>
       <c r="D34">
-        <v>264.328017401161</v>
+        <v>264.2557321436792</v>
       </c>
       <c r="E34">
-        <v>0.02100949874008451</v>
+        <v>0.02068306004908102</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2">
-        <v>31479</v>
+        <v>31478.58333333333</v>
       </c>
       <c r="B35">
-        <v>0.04558333333333327</v>
+        <v>0.04275000000000001</v>
       </c>
       <c r="C35">
-        <v>0.08145003708568765</v>
+        <v>0.07833167191449775</v>
       </c>
       <c r="D35">
-        <v>264.4100586178439</v>
+        <v>264.3327776061171</v>
       </c>
       <c r="E35">
-        <v>0.02137999513610354</v>
+        <v>0.02103099572479391</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2">
-        <v>31510</v>
+        <v>31509</v>
       </c>
       <c r="B36">
-        <v>0.04604166666666661</v>
+        <v>0.04312500000000001</v>
       </c>
       <c r="C36">
-        <v>0.0540348385161451</v>
+        <v>0.07331847621958332</v>
       </c>
       <c r="D36">
-        <v>264.4915086549296</v>
+        <v>264.4111092780316</v>
       </c>
       <c r="E36">
-        <v>0.02174782177758914</v>
+        <v>0.02138473989524693</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2">
-        <v>31571</v>
+        <v>31569.83333333333</v>
       </c>
       <c r="B37">
-        <v>0.04649999999999994</v>
+        <v>0.04350000000000001</v>
       </c>
       <c r="C37">
-        <v>0.91148249997525</v>
+        <v>0.8975378949063497</v>
       </c>
       <c r="D37">
-        <v>263.4790900049385</v>
+        <v>263.4399123324016</v>
       </c>
       <c r="E37">
-        <v>0.0171757606082154</v>
+        <v>0.01699883506924602</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2">
-        <v>31601</v>
+        <v>31600.25</v>
       </c>
       <c r="B38">
-        <v>0.04695833333333327</v>
+        <v>0.04387500000000001</v>
       </c>
       <c r="C38">
-        <v>0.281988160954711</v>
+        <v>0.2762811811343227</v>
       </c>
       <c r="D38">
-        <v>264.3905725049137</v>
+        <v>264.337450227308</v>
       </c>
       <c r="E38">
-        <v>0.02129199626303771</v>
+        <v>0.02105209718307488</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2">
-        <v>31632</v>
+        <v>31630.66666666667</v>
       </c>
       <c r="B39">
-        <v>0.0474166666666666</v>
+        <v>0.04425000000000001</v>
       </c>
       <c r="C39">
-        <v>0.129444757350484</v>
+        <v>0.1265835878132293</v>
       </c>
       <c r="D39">
-        <v>264.6725606658684</v>
+        <v>264.6137314084423</v>
       </c>
       <c r="E39">
-        <v>0.02256544882234755</v>
+        <v>0.02229977714245146</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2">
-        <v>31663</v>
+        <v>31661.08333333333</v>
       </c>
       <c r="B40">
-        <v>0.04787499999999993</v>
+        <v>0.04462500000000001</v>
       </c>
       <c r="C40">
-        <v>0.09278948265568943</v>
+        <v>0.09071938595616302</v>
       </c>
       <c r="D40">
-        <v>264.8020054232189</v>
+        <v>264.7403149962555</v>
       </c>
       <c r="E40">
-        <v>0.02315001860350118</v>
+        <v>0.02287142594260533</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2">
-        <v>31693</v>
+        <v>31691.5</v>
       </c>
       <c r="B41">
-        <v>0.04833333333333326</v>
+        <v>0.04500000000000001</v>
       </c>
       <c r="C41">
-        <v>0.08528420708694284</v>
+        <v>0.08152618015424196</v>
       </c>
       <c r="D41">
-        <v>264.8947949058746</v>
+        <v>264.8310343822117</v>
       </c>
       <c r="E41">
-        <v>0.02356905394088845</v>
+        <v>0.02328111276716464</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2">
-        <v>31724</v>
+        <v>31721.91666666667</v>
       </c>
       <c r="B42">
-        <v>0.04879166666666659</v>
+        <v>0.04537500000000001</v>
       </c>
       <c r="C42">
-        <v>0.08301208209195465</v>
+        <v>0.07783177502437866</v>
       </c>
       <c r="D42">
-        <v>264.9800791129616</v>
+        <v>264.9125605623659</v>
       </c>
       <c r="E42">
-        <v>0.02395419561285039</v>
+        <v>0.02364928326913423</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2">
-        <v>31754</v>
+        <v>31752.33333333333</v>
       </c>
       <c r="B43">
-        <v>0.04924999999999993</v>
+        <v>0.04575000000000001</v>
       </c>
       <c r="C43">
-        <v>0.08352370698730738</v>
+        <v>0.07890318642216698</v>
       </c>
       <c r="D43">
-        <v>265.0630911950535</v>
+        <v>264.9903923373903</v>
       </c>
       <c r="E43">
-        <v>0.0243290764164833</v>
+        <v>0.02400076991582486</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2">
-        <v>31785</v>
+        <v>31782.75</v>
       </c>
       <c r="B44">
-        <v>0.04970833333333326</v>
+        <v>0.04612500000000001</v>
       </c>
       <c r="C44">
-        <v>0.08404388793417183</v>
+        <v>0.07921275357625746</v>
       </c>
       <c r="D44">
-        <v>265.1466149020408</v>
+        <v>265.0692955238125</v>
       </c>
       <c r="E44">
-        <v>0.02470626770730178</v>
+        <v>0.02435709503368383</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2">
-        <v>31816</v>
+        <v>31813.16666666667</v>
       </c>
       <c r="B45">
-        <v>0.05016666666666659</v>
+        <v>0.04650000000000001</v>
       </c>
       <c r="C45">
-        <v>0.08536462415531787</v>
+        <v>0.07989350726529665</v>
       </c>
       <c r="D45">
-        <v>265.230658789975</v>
+        <v>265.1485082773887</v>
       </c>
       <c r="E45">
-        <v>0.02508580812425307</v>
+        <v>0.02471481815025062</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2">
-        <v>31844</v>
+        <v>31843.58333333333</v>
       </c>
       <c r="B46">
-        <v>0.05062499999999992</v>
+        <v>0.04687500000000001</v>
       </c>
       <c r="C46">
-        <v>0.06016232353988471</v>
+        <v>0.05167126783362619</v>
       </c>
       <c r="D46">
-        <v>265.3160234141303</v>
+        <v>265.228401784654</v>
       </c>
       <c r="E46">
-        <v>0.02547131295799172</v>
+        <v>0.02507561553605127</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2">
-        <v>31905</v>
+        <v>31904.41666666667</v>
       </c>
       <c r="B47">
-        <v>0.05108333333333325</v>
+        <v>0.04725000000000001</v>
       </c>
       <c r="C47">
-        <v>1.080019576750146</v>
+        <v>1.05435836455581</v>
       </c>
       <c r="D47">
-        <v>264.0261042234227</v>
+        <v>263.9571694291507</v>
       </c>
       <c r="E47">
-        <v>0.01964606522720792</v>
+        <v>0.01933475715706029</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2">
-        <v>31936</v>
+        <v>31934.83333333333</v>
       </c>
       <c r="B48">
-        <v>0.05154166666666658</v>
+        <v>0.04762500000000001</v>
       </c>
       <c r="C48">
-        <v>0.3156716324392619</v>
+        <v>0.3037407506801628</v>
       </c>
       <c r="D48">
-        <v>265.1061238001729</v>
+        <v>265.0115277937065</v>
       </c>
       <c r="E48">
-        <v>0.02452341074930593</v>
+        <v>0.024096217188671</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2">
-        <v>31966</v>
+        <v>31965.25</v>
       </c>
       <c r="B49">
-        <v>0.05199999999999991</v>
+        <v>0.04800000000000001</v>
       </c>
       <c r="C49">
-        <v>0.1260570026404366</v>
+        <v>0.1183837365827003</v>
       </c>
       <c r="D49">
-        <v>265.4217954326122</v>
+        <v>265.3152685443866</v>
       </c>
       <c r="E49">
-        <v>0.02594897715205938</v>
+        <v>0.02546790398222569</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2">
-        <v>31997</v>
+        <v>31995.66666666667</v>
       </c>
       <c r="B50">
-        <v>0.05245833333333325</v>
+        <v>0.04837500000000002</v>
       </c>
       <c r="C50">
-        <v>0.07669956028826164</v>
+        <v>0.07144299549975131</v>
       </c>
       <c r="D50">
-        <v>265.5478524352526</v>
+        <v>265.4336522809693</v>
       </c>
       <c r="E50">
-        <v>0.02651824790473171</v>
+        <v>0.02600252242798405</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2">
-        <v>32028</v>
+        <v>32026.08333333333</v>
       </c>
       <c r="B51">
-        <v>0.05291666666666658</v>
+        <v>0.04875000000000002</v>
       </c>
       <c r="C51">
-        <v>0.06416821351274393</v>
+        <v>0.05904983962716415</v>
       </c>
       <c r="D51">
-        <v>265.6245519955409</v>
+        <v>265.5050952764691</v>
       </c>
       <c r="E51">
-        <v>0.02686462149366661</v>
+        <v>0.02632515748172492</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2">
-        <v>32058</v>
+        <v>32056.5</v>
       </c>
       <c r="B52">
-        <v>0.05337499999999991</v>
+        <v>0.04912500000000002</v>
       </c>
       <c r="C52">
-        <v>0.06388777329664208</v>
+        <v>0.05570617525791022</v>
       </c>
       <c r="D52">
-        <v>265.6887202090536</v>
+        <v>265.5641451160963</v>
       </c>
       <c r="E52">
-        <v>0.02715440378611277</v>
+        <v>0.02659182530616642</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2">
-        <v>32089</v>
+        <v>32086.91666666667</v>
       </c>
       <c r="B53">
-        <v>0.05383333333333324</v>
+        <v>0.04950000000000002</v>
       </c>
       <c r="C53">
-        <v>0.0626807837686556</v>
+        <v>0.05569454159319775</v>
       </c>
       <c r="D53">
-        <v>265.7526079823502</v>
+        <v>265.6198512913542</v>
       </c>
       <c r="E53">
-        <v>0.02744291961648579</v>
+        <v>0.02684339321317139</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2">
-        <v>32119</v>
+        <v>32117.33333333333</v>
       </c>
       <c r="B54">
-        <v>0.05429166666666657</v>
+        <v>0.04987500000000002</v>
       </c>
       <c r="C54">
-        <v>0.0607206303006933</v>
+        <v>0.05377025213658726</v>
       </c>
       <c r="D54">
-        <v>265.8152887661189</v>
+        <v>265.6755458329474</v>
       </c>
       <c r="E54">
-        <v>0.02772598470772765</v>
+        <v>0.02709490858279301</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2">
-        <v>32150</v>
+        <v>32147.75</v>
       </c>
       <c r="B55">
-        <v>0.0547499999999999</v>
+        <v>0.05025000000000002</v>
       </c>
       <c r="C55">
-        <v>0.06053060012641254</v>
+        <v>0.0536651513398283</v>
       </c>
       <c r="D55">
-        <v>265.8760093964196</v>
+        <v>265.729316085084</v>
       </c>
       <c r="E55">
-        <v>0.02800019778744529</v>
+        <v>0.02733773390200581</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2">
-        <v>32181</v>
+        <v>32178.16666666667</v>
       </c>
       <c r="B56">
-        <v>0.05520833333333323</v>
+        <v>0.05062500000000002</v>
       </c>
       <c r="C56">
-        <v>0.0607833220556131</v>
+        <v>0.05372541344513593</v>
       </c>
       <c r="D56">
-        <v>265.936539996546</v>
+        <v>265.7829812364238</v>
       </c>
       <c r="E56">
-        <v>0.02827355269492284</v>
+        <v>0.02758008458824764</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2">
-        <v>32210</v>
+        <v>32208.58333333333</v>
       </c>
       <c r="B57">
-        <v>0.05566666666666657</v>
+        <v>0.05100000000000002</v>
       </c>
       <c r="C57">
-        <v>-0.7949311580347285</v>
+        <v>-0.3258022958318634</v>
       </c>
       <c r="D57">
-        <v>265.9973233186016</v>
+        <v>265.8367066498689</v>
       </c>
       <c r="E57">
-        <v>0.02854804888927719</v>
+        <v>0.02782270741688007</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2">
-        <v>32271</v>
+        <v>32269.41666666667</v>
       </c>
       <c r="B58">
-        <v>0.0561249999999999</v>
+        <v>0.05137500000000002</v>
       </c>
       <c r="C58">
-        <v>0.9714709399851245</v>
+        <v>1.073671410254065</v>
       </c>
       <c r="D58">
-        <v>263.7285901987012</v>
+        <v>264.0278294741912</v>
       </c>
       <c r="E58">
-        <v>0.0183024981961331</v>
+        <v>0.01965385642311871</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2">
-        <v>32302</v>
+        <v>32299.83333333333</v>
       </c>
       <c r="B59">
-        <v>0.05658333333333323</v>
+        <v>0.05175000000000002</v>
       </c>
       <c r="C59">
-        <v>0.2800621243441128</v>
+        <v>0.3019505282175032</v>
       </c>
       <c r="D59">
-        <v>264.7000611386864</v>
+        <v>265.1015008844453</v>
       </c>
       <c r="E59">
-        <v>0.02268964037483538</v>
+        <v>0.02450253375984343</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2">
-        <v>32363</v>
+        <v>32360.66666666667</v>
       </c>
       <c r="B60">
-        <v>0.05704166666666656</v>
+        <v>0.05212500000000002</v>
       </c>
       <c r="C60">
-        <v>0.9985082383151394</v>
+        <v>1.098418247895665</v>
       </c>
       <c r="D60">
-        <v>263.8149084194674</v>
+        <v>264.0978991005857</v>
       </c>
       <c r="E60">
-        <v>0.01869230945195889</v>
+        <v>0.01997028937108295</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2">
-        <v>32394</v>
+        <v>32391.08333333333</v>
       </c>
       <c r="B61">
-        <v>0.05749999999999989</v>
+        <v>0.05250000000000002</v>
       </c>
       <c r="C61">
-        <v>0.2897141910592609</v>
+        <v>0.3092665440224209</v>
       </c>
       <c r="D61">
-        <v>264.8134166577826</v>
+        <v>265.1963173484813</v>
       </c>
       <c r="E61">
-        <v>0.02320155149697701</v>
+        <v>0.02493072290219119</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2">
-        <v>32455</v>
+        <v>32451.91666666667</v>
       </c>
       <c r="B62">
-        <v>0.05795833333333322</v>
+        <v>0.05287500000000002</v>
       </c>
       <c r="C62">
-        <v>1.028248152728338</v>
+        <v>1.12288810633936</v>
       </c>
       <c r="D62">
-        <v>263.9000967064911</v>
+        <v>264.1684372823217</v>
       </c>
       <c r="E62">
-        <v>0.01907701795094797</v>
+        <v>0.02028883830504082</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="2">
-        <v>32485</v>
+        <v>32482.33333333333</v>
       </c>
       <c r="B63">
-        <v>0.05841666666666655</v>
+        <v>0.05325000000000002</v>
       </c>
       <c r="C63">
-        <v>0.3033869920013785</v>
+        <v>0.3261510677734805</v>
       </c>
       <c r="D63">
-        <v>264.9283448592195</v>
+        <v>265.2913253886611</v>
       </c>
       <c r="E63">
-        <v>0.02372056481924262</v>
+        <v>0.02535977719834432</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="2">
-        <v>32516</v>
+        <v>32512.75</v>
       </c>
       <c r="B64">
-        <v>0.05887499999999989</v>
+        <v>0.05362500000000002</v>
       </c>
       <c r="C64">
-        <v>0.1213831496720559</v>
+        <v>0.1253393088821895</v>
       </c>
       <c r="D64">
-        <v>265.2317318512208</v>
+        <v>265.6174764564346</v>
       </c>
       <c r="E64">
-        <v>0.02509065404610022</v>
+        <v>0.02683266850899928</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2">
-        <v>32547</v>
+        <v>32543.16666666667</v>
       </c>
       <c r="B65">
-        <v>0.05933333333333322</v>
+        <v>0.05400000000000002</v>
       </c>
       <c r="C65">
-        <v>0.07618614958369108</v>
+        <v>0.07406258297737622</v>
       </c>
       <c r="D65">
-        <v>265.3531150008929</v>
+        <v>265.7428157653168</v>
       </c>
       <c r="E65">
-        <v>0.02563881777781032</v>
+        <v>0.02739869817186786</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="2">
-        <v>32575</v>
+        <v>32573.58333333333</v>
       </c>
       <c r="B66">
-        <v>0.05979166666666655</v>
+        <v>0.05437500000000002</v>
       </c>
       <c r="C66">
-        <v>0.06550400709988935</v>
+        <v>0.06131125660886028</v>
       </c>
       <c r="D66">
-        <v>265.4293011504766</v>
+        <v>265.8168783482942</v>
       </c>
       <c r="E66">
-        <v>0.02598287281488278</v>
+        <v>0.0277331632271465</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="2">
-        <v>32606</v>
+        <v>32604</v>
       </c>
       <c r="B67">
-        <v>0.06024999999999988</v>
+        <v>0.05475000000000002</v>
       </c>
       <c r="C67">
-        <v>0.06325743695015262</v>
+        <v>0.05949998303549364</v>
       </c>
       <c r="D67">
-        <v>265.4948051575765</v>
+        <v>265.878189604903</v>
       </c>
       <c r="E67">
-        <v>0.02627868752286196</v>
+        <v>0.02801004356275595</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="2">
-        <v>32636</v>
+        <v>32634.41666666667</v>
       </c>
       <c r="B68">
-        <v>0.06070833333333321</v>
+        <v>0.05512500000000002</v>
       </c>
       <c r="C68">
-        <v>0.05819852115246249</v>
+        <v>0.0490905436633966</v>
       </c>
       <c r="D68">
-        <v>265.5580625945266</v>
+        <v>265.9376895879385</v>
       </c>
       <c r="E68">
-        <v>0.02656435676765159</v>
+        <v>0.02827874422529065</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="2">
-        <v>32697</v>
+        <v>32695.25</v>
       </c>
       <c r="B69">
-        <v>0.06116666666666654</v>
+        <v>0.05550000000000002</v>
       </c>
       <c r="C69">
-        <v>1.129019064949603</v>
+        <v>1.213538529142852</v>
       </c>
       <c r="D69">
-        <v>264.190460345987</v>
+        <v>264.422791719075</v>
       </c>
       <c r="E69">
-        <v>0.02038829399386657</v>
+        <v>0.02143749755143828</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="2">
-        <v>32728</v>
+        <v>32725.66666666667</v>
       </c>
       <c r="B70">
-        <v>0.06162499999999987</v>
+        <v>0.05587500000000002</v>
       </c>
       <c r="C70">
-        <v>0.3337013418390598</v>
+        <v>0.3587513553129611</v>
       </c>
       <c r="D70">
-        <v>265.3194794109367</v>
+        <v>265.6363302482179</v>
       </c>
       <c r="E70">
-        <v>0.02548692016633382</v>
+        <v>0.02691781183316519</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="2">
-        <v>32759</v>
+        <v>32756.08333333333</v>
       </c>
       <c r="B71">
-        <v>0.06208333333333321</v>
+        <v>0.05625000000000002</v>
       </c>
       <c r="C71">
-        <v>0.1298741274254098</v>
+        <v>0.136515315999759</v>
       </c>
       <c r="D71">
-        <v>265.6531807527757</v>
+        <v>265.9950816035308</v>
       </c>
       <c r="E71">
-        <v>0.02699390835467234</v>
+        <v>0.02853792535152138</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="2">
-        <v>32789</v>
+        <v>32786.5</v>
       </c>
       <c r="B72">
-        <v>0.06254166666666654</v>
+        <v>0.05662500000000002</v>
       </c>
       <c r="C72">
-        <v>0.07944433463057976</v>
+        <v>0.07765946292931858</v>
       </c>
       <c r="D72">
-        <v>265.7830548802011</v>
+        <v>266.1315969195306</v>
       </c>
       <c r="E72">
-        <v>0.02758041716198551</v>
+        <v>0.02915442562570402</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="2">
-        <v>32820</v>
+        <v>32816.91666666666</v>
       </c>
       <c r="B73">
-        <v>0.06299999999999988</v>
+        <v>0.05700000000000002</v>
       </c>
       <c r="C73">
-        <v>0.066111478543462</v>
+        <v>0.06191882557811823</v>
       </c>
       <c r="D73">
-        <v>265.8624992148317</v>
+        <v>266.2092563824599</v>
       </c>
       <c r="E73">
-        <v>0.02793918609368627</v>
+        <v>0.02950513411462488</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="2">
-        <v>32850</v>
+        <v>32847.33333333334</v>
       </c>
       <c r="B74">
-        <v>0.06345833333333321</v>
+        <v>0.05737500000000002</v>
       </c>
       <c r="C74">
-        <v>0.06329735390841051</v>
+        <v>0.05717666325313076</v>
       </c>
       <c r="D74">
-        <v>265.9286106933752</v>
+        <v>266.271175208038</v>
       </c>
       <c r="E74">
-        <v>0.02823774412983174</v>
+        <v>0.02978475821882458</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="2">
-        <v>32881</v>
+        <v>32877.75</v>
       </c>
       <c r="B75">
-        <v>0.06391666666666655</v>
+        <v>0.05775000000000002</v>
       </c>
       <c r="C75">
-        <v>0.05929775369372692</v>
+        <v>0.04894698049020008</v>
       </c>
       <c r="D75">
-        <v>265.9919080472836</v>
+        <v>266.3283518712911</v>
       </c>
       <c r="E75">
-        <v>0.02852359363875908</v>
+        <v>0.03004296681845518</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="2">
-        <v>32940</v>
+        <v>32938.58333333334</v>
       </c>
       <c r="B76">
-        <v>0.06437499999999989</v>
+        <v>0.05812500000000002</v>
       </c>
       <c r="C76">
-        <v>1.229312957721163</v>
+        <v>1.29594751404511</v>
       </c>
       <c r="D76">
-        <v>264.4766543977652</v>
+        <v>264.6744700945729</v>
       </c>
       <c r="E76">
-        <v>0.02168074026700861</v>
+        <v>0.02257407176191465</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="2">
-        <v>33001</v>
+        <v>32999.41666666666</v>
       </c>
       <c r="B77">
-        <v>0.06483333333333323</v>
+        <v>0.05850000000000002</v>
       </c>
       <c r="C77">
-        <v>1.249547720390751</v>
+        <v>1.319385708037544</v>
       </c>
       <c r="D77">
-        <v>264.5222486963013</v>
+        <v>264.7094907442457</v>
       </c>
       <c r="E77">
-        <v>0.02188664315301687</v>
+        <v>0.02273222427372057</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="2">
-        <v>33032</v>
+        <v>33029.83333333334</v>
       </c>
       <c r="B78">
-        <v>0.06529166666666657</v>
+        <v>0.05887500000000002</v>
       </c>
       <c r="C78">
-        <v>0.3730063015372025</v>
+        <v>0.396994486316089</v>
       </c>
       <c r="D78">
-        <v>265.771796416692</v>
+        <v>266.0288764522833</v>
       </c>
       <c r="E78">
-        <v>0.02752957417935474</v>
+        <v>0.02869054217234668</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="2">
-        <v>33062</v>
+        <v>33060.25</v>
       </c>
       <c r="B79">
-        <v>0.06574999999999991</v>
+        <v>0.05925000000000002</v>
       </c>
       <c r="C79">
-        <v>0.1434178509005051</v>
+        <v>0.148504673336106</v>
       </c>
       <c r="D79">
-        <v>266.1448027182292</v>
+        <v>266.4258709385994</v>
       </c>
       <c r="E79">
-        <v>0.02921406273278552</v>
+        <v>0.03048336085990946</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="2">
-        <v>33093</v>
+        <v>33090.66666666666</v>
       </c>
       <c r="B80">
-        <v>0.06620833333333324</v>
+        <v>0.05962500000000003</v>
       </c>
       <c r="C80">
-        <v>0.08415010476983298</v>
+        <v>0.08313392534455488</v>
       </c>
       <c r="D80">
-        <v>266.2882205691297</v>
+        <v>266.5743756119355</v>
       </c>
       <c r="E80">
-        <v>0.0298617347083096</v>
+        <v>0.0311540048177589</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="2">
-        <v>33124</v>
+        <v>33121.08333333334</v>
       </c>
       <c r="B81">
-        <v>0.06666666666666658</v>
+        <v>0.06000000000000003</v>
       </c>
       <c r="C81">
-        <v>0.06883728042282655</v>
+        <v>0.06435457205691364</v>
       </c>
       <c r="D81">
-        <v>266.3723706738996</v>
+        <v>266.65750953728</v>
       </c>
       <c r="E81">
-        <v>0.03024175479824005</v>
+        <v>0.03152943586293852</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="2">
-        <v>33154</v>
+        <v>33151.5</v>
       </c>
       <c r="B82">
-        <v>0.06712499999999992</v>
+        <v>0.06037500000000003</v>
       </c>
       <c r="C82">
-        <v>0.0645953803178827</v>
+        <v>0.05881205803189005</v>
       </c>
       <c r="D82">
-        <v>266.4412079543224</v>
+        <v>266.7218641093369</v>
       </c>
       <c r="E82">
-        <v>0.0305526224979108</v>
+        <v>0.03182005974662098</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="2">
-        <v>33185</v>
+        <v>33181.91666666666</v>
       </c>
       <c r="B83">
-        <v>0.06758333333333326</v>
+        <v>0.06075000000000003</v>
       </c>
       <c r="C83">
-        <v>0.06410930194977027</v>
+        <v>0.0565354103395066</v>
       </c>
       <c r="D83">
-        <v>266.5058033346403</v>
+        <v>266.7806761673688</v>
       </c>
       <c r="E83">
-        <v>0.03084433386659703</v>
+        <v>0.03208565375441701</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="2">
-        <v>33215</v>
+        <v>33212.33333333334</v>
       </c>
       <c r="B84">
-        <v>0.0680416666666666</v>
+        <v>0.06112500000000003</v>
       </c>
       <c r="C84">
-        <v>0.06411089136838655</v>
+        <v>0.05610703139348061</v>
       </c>
       <c r="D84">
-        <v>266.5699126365901</v>
+        <v>266.8372115777083</v>
       </c>
       <c r="E84">
-        <v>0.03113385011567323</v>
+        <v>0.0323409664694782</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="2">
-        <v>33246</v>
+        <v>33242.75</v>
       </c>
       <c r="B85">
-        <v>0.06849999999999994</v>
+        <v>0.06150000000000003</v>
       </c>
       <c r="C85">
-        <v>0.06483197510658556</v>
+        <v>0.05511731397268704</v>
       </c>
       <c r="D85">
-        <v>266.6340235279584</v>
+        <v>266.8933186091018</v>
       </c>
       <c r="E85">
-        <v>0.03142337354253014</v>
+        <v>0.03259434463429683</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="2">
-        <v>33277</v>
+        <v>33273.16666666666</v>
       </c>
       <c r="B86">
-        <v>0.06895833333333327</v>
+        <v>0.06187500000000003</v>
       </c>
       <c r="C86">
-        <v>0.06445784365951113</v>
+        <v>0.05650100091452259</v>
       </c>
       <c r="D86">
-        <v>266.698855503065</v>
+        <v>266.9484359230745</v>
       </c>
       <c r="E86">
-        <v>0.03171615336826845</v>
+        <v>0.03284325325621617</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="2">
-        <v>33305</v>
+        <v>33303.58333333334</v>
       </c>
       <c r="B87">
-        <v>0.06941666666666661</v>
+        <v>0.06225000000000003</v>
       </c>
       <c r="C87">
-        <v>0.06375244257094437</v>
+        <v>0.05676646017877829</v>
       </c>
       <c r="D87">
-        <v>266.7633133467245</v>
+        <v>267.004936923989</v>
       </c>
       <c r="E87">
-        <v>0.03200724362431989</v>
+        <v>0.03309841057904332</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="2">
-        <v>33336</v>
+        <v>33334</v>
       </c>
       <c r="B88">
-        <v>0.06987499999999995</v>
+        <v>0.06262500000000003</v>
       </c>
       <c r="C88">
-        <v>0.06199103701646891</v>
+        <v>0.05827534052014016</v>
       </c>
       <c r="D88">
-        <v>266.8270657892955</v>
+        <v>267.0617033841678</v>
       </c>
       <c r="E88">
-        <v>0.03229514830400347</v>
+        <v>0.03335476671028272</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="2">
-        <v>33366</v>
+        <v>33364.41666666666</v>
       </c>
       <c r="B89">
-        <v>0.07033333333333329</v>
+        <v>0.06300000000000003</v>
       </c>
       <c r="C89">
-        <v>0.0624083359175529</v>
+        <v>0.05697156024359629</v>
       </c>
       <c r="D89">
-        <v>266.889056826312</v>
+        <v>267.1199787246879</v>
       </c>
       <c r="E89">
-        <v>0.03257509851352856</v>
+        <v>0.03361793691316908</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="2">
-        <v>33397</v>
+        <v>33394.83333333334</v>
       </c>
       <c r="B90">
-        <v>0.07079166666666663</v>
+        <v>0.06337500000000003</v>
       </c>
       <c r="C90">
-        <v>0.06311421089094438</v>
+        <v>0.05597215117040832</v>
       </c>
       <c r="D90">
-        <v>266.9514651622295</v>
+        <v>267.1769502849315</v>
       </c>
       <c r="E90">
-        <v>0.0328569332360481</v>
+        <v>0.03387521927195476</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="2">
-        <v>33427</v>
+        <v>33425.25</v>
       </c>
       <c r="B91">
-        <v>0.07124999999999997</v>
+        <v>0.06375000000000003</v>
       </c>
       <c r="C91">
-        <v>0.05965977063806349</v>
+        <v>0.04870844378478978</v>
       </c>
       <c r="D91">
-        <v>267.0145793731205</v>
+        <v>267.2329224361019</v>
       </c>
       <c r="E91">
-        <v>0.03314195567498949</v>
+        <v>0.03412798832054425</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="2">
-        <v>33519</v>
+        <v>33516.5</v>
       </c>
       <c r="B92">
-        <v>0.0717083333333333</v>
+        <v>0.06412500000000003</v>
       </c>
       <c r="C92">
-        <v>1.476431826416615</v>
+        <v>1.524982115772332</v>
       </c>
       <c r="D92">
-        <v>265.1303511145455</v>
+        <v>265.2374172359175</v>
       </c>
       <c r="E92">
-        <v>0.02463282078761605</v>
+        <v>0.02511632912291254</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="2">
-        <v>33550</v>
+        <v>33546.91666666666</v>
       </c>
       <c r="B93">
-        <v>0.07216666666666664</v>
+        <v>0.06450000000000003</v>
       </c>
       <c r="C93">
-        <v>0.456932931270444</v>
+        <v>0.4743536305225007</v>
       </c>
       <c r="D93">
-        <v>266.6067829409621</v>
+        <v>266.7623993516899</v>
       </c>
       <c r="E93">
-        <v>0.03130035562890528</v>
+        <v>0.03200311604211149</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="2">
-        <v>33580</v>
+        <v>33577.33333333334</v>
       </c>
       <c r="B94">
-        <v>0.07262499999999998</v>
+        <v>0.06487500000000003</v>
       </c>
       <c r="C94">
-        <v>0.1727923523081927</v>
+        <v>0.1789972944447982</v>
       </c>
       <c r="D94">
-        <v>267.0637158722326</v>
+        <v>267.2367529822124</v>
       </c>
       <c r="E94">
-        <v>0.03336385506373694</v>
+        <v>0.03414528698560656</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="2">
-        <v>33611</v>
+        <v>33607.75</v>
       </c>
       <c r="B95">
-        <v>0.07308333333333332</v>
+        <v>0.06525000000000003</v>
       </c>
       <c r="C95">
-        <v>0.09631236367101792</v>
+        <v>0.08593647928910286</v>
       </c>
       <c r="D95">
-        <v>267.2365082245408</v>
+        <v>267.4157502766571</v>
       </c>
       <c r="E95">
-        <v>0.03414418166514832</v>
+        <v>0.03495363497421889</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="2">
-        <v>33642</v>
+        <v>33638.16666666666</v>
       </c>
       <c r="B96">
-        <v>0.07354166666666666</v>
+        <v>0.06562500000000003</v>
       </c>
       <c r="C96">
-        <v>0.07317824335950718</v>
+        <v>0.0661964537816857</v>
       </c>
       <c r="D96">
-        <v>267.3328205882118</v>
+        <v>267.5016867559463</v>
       </c>
       <c r="E96">
-        <v>0.03457912625854815</v>
+        <v>0.03534172229362362</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="2">
-        <v>33671</v>
+        <v>33668.58333333334</v>
       </c>
       <c r="B97">
-        <v>0.074</v>
+        <v>0.06600000000000003</v>
       </c>
       <c r="C97">
-        <v>0.06445712624622502</v>
+        <v>0.05279433186092319</v>
       </c>
       <c r="D97">
-        <v>267.4059988315713</v>
+        <v>267.5678832097279</v>
       </c>
       <c r="E97">
-        <v>0.03490959765485235</v>
+        <v>0.03564066407614432</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="2">
-        <v>33732</v>
+        <v>33729.41666666666</v>
       </c>
       <c r="B98">
-        <v>0.07445833333333333</v>
+        <v>0.06637500000000003</v>
       </c>
       <c r="C98">
-        <v>1.574001883426376</v>
+        <v>1.611065964479621</v>
       </c>
       <c r="D98">
-        <v>265.3690767605491</v>
+        <v>265.4501507443838</v>
       </c>
       <c r="E98">
-        <v>0.02571090074617476</v>
+        <v>0.02607702913914765</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="2">
-        <v>33763</v>
+        <v>33759.83333333334</v>
       </c>
       <c r="B99">
-        <v>0.07491666666666667</v>
+        <v>0.06675000000000003</v>
       </c>
       <c r="C99">
-        <v>0.4950268054786875</v>
+        <v>0.5087105507124079</v>
       </c>
       <c r="D99">
-        <v>266.9430786439755</v>
+        <v>267.0612167088634</v>
       </c>
       <c r="E99">
-        <v>0.0328190598973301</v>
+        <v>0.03335256889492105</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="2">
-        <v>33793</v>
+        <v>33790.25</v>
       </c>
       <c r="B100">
-        <v>0.07537500000000001</v>
+        <v>0.06712500000000003</v>
       </c>
       <c r="C100">
-        <v>0.1925776989169208</v>
+        <v>0.1825163532771512</v>
       </c>
       <c r="D100">
-        <v>267.4381054494542</v>
+        <v>267.5699272595758</v>
       </c>
       <c r="E100">
-        <v>0.03505459046084571</v>
+        <v>0.0356498949619421</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="2">
-        <v>33824</v>
+        <v>33820.66666666666</v>
       </c>
       <c r="B101">
-        <v>0.07583333333333335</v>
+        <v>0.06750000000000003</v>
       </c>
       <c r="C101">
-        <v>0.1029590768275739</v>
+        <v>0.09466089648390152</v>
       </c>
       <c r="D101">
-        <v>267.6306831483711</v>
+        <v>267.752443612853</v>
       </c>
       <c r="E101">
-        <v>0.03592426726827423</v>
+        <v>0.03647413494566965</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="2">
-        <v>33855</v>
+        <v>33851.08333333334</v>
       </c>
       <c r="B102">
-        <v>0.07629166666666669</v>
+        <v>0.06787500000000003</v>
       </c>
       <c r="C102">
-        <v>0.07560920482433175</v>
+        <v>0.07063909676037383</v>
       </c>
       <c r="D102">
-        <v>267.7336422251987</v>
+        <v>267.8471045093369</v>
       </c>
       <c r="E102">
-        <v>0.03638922827743974</v>
+        <v>0.03690162154824865</v>
       </c>
     </row>
   </sheetData>
@@ -2150,7 +2150,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2181,495 +2181,614 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>33885</v>
+        <v>33911.91666666666</v>
       </c>
       <c r="B2">
-        <v>0.07675000000000003</v>
+        <v>0.06862500000000003</v>
       </c>
       <c r="C2">
-        <v>-1.321870552647852</v>
+        <v>-0.3519853857835642</v>
       </c>
       <c r="D2">
-        <v>267.809251430023</v>
+        <v>266.5943176828133</v>
       </c>
       <c r="E2">
-        <v>0.03673067784420499</v>
+        <v>0.03124406278725433</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>33916</v>
+        <v>33942.33333333334</v>
       </c>
       <c r="B3">
-        <v>0.07720833333333336</v>
+        <v>0.06900000000000003</v>
       </c>
       <c r="C3">
-        <v>-0.3337857789060763</v>
+        <v>-0.06001121969347878</v>
       </c>
       <c r="D3">
-        <v>266.4873808773751</v>
+        <v>266.2423322970297</v>
       </c>
       <c r="E3">
-        <v>0.03076113843997461</v>
+        <v>0.02965450424391631</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>33946</v>
+        <v>33972.75</v>
       </c>
       <c r="B4">
-        <v>0.0776666666666667</v>
+        <v>0.06937500000000003</v>
       </c>
       <c r="C4">
-        <v>-0.05193031826252081</v>
+        <v>0.02446254093672451</v>
       </c>
       <c r="D4">
-        <v>266.1535950984691</v>
+        <v>266.1823210773363</v>
       </c>
       <c r="E4">
-        <v>0.02925376893563076</v>
+        <v>0.0293834948474678</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>33977</v>
+        <v>34003.16666666666</v>
       </c>
       <c r="B5">
-        <v>0.07812500000000004</v>
+        <v>0.06975000000000003</v>
       </c>
       <c r="C5">
-        <v>0.02798452484421432</v>
+        <v>0.04798312370087388</v>
       </c>
       <c r="D5">
-        <v>266.1016647802065</v>
+        <v>266.206783618273</v>
       </c>
       <c r="E5">
-        <v>0.02901925271880345</v>
+        <v>0.02949396716395665</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>34008</v>
+        <v>34033.58333333334</v>
       </c>
       <c r="B6">
-        <v>0.07858333333333338</v>
+        <v>0.07012500000000003</v>
       </c>
       <c r="C6">
-        <v>0.0525885856086461</v>
+        <v>0.05375077600922396</v>
       </c>
       <c r="D6">
-        <v>266.1296493050507</v>
+        <v>266.2547667419739</v>
       </c>
       <c r="E6">
-        <v>0.02914563023998474</v>
+        <v>0.02971065793378791</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2">
-        <v>34036</v>
+        <v>34064</v>
       </c>
       <c r="B7">
-        <v>0.07904166666666672</v>
+        <v>0.07050000000000003</v>
       </c>
       <c r="C7">
-        <v>0.05786109520568061</v>
+        <v>0.05545922149292437</v>
       </c>
       <c r="D7">
-        <v>266.1822378906594</v>
+        <v>266.3085175179831</v>
       </c>
       <c r="E7">
-        <v>0.02938311917819786</v>
+        <v>0.02995339529922232</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2">
-        <v>34067</v>
+        <v>34094.41666666666</v>
       </c>
       <c r="B8">
-        <v>0.07950000000000006</v>
+        <v>0.07087500000000004</v>
       </c>
       <c r="C8">
-        <v>0.06203646546782693</v>
+        <v>0.05677885489558321</v>
       </c>
       <c r="D8">
-        <v>266.2400989858651</v>
+        <v>266.363976739476</v>
       </c>
       <c r="E8">
-        <v>0.02964441865802242</v>
+        <v>0.03020384796825756</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
-        <v>34097</v>
+        <v>34124.83333333334</v>
       </c>
       <c r="B9">
-        <v>0.0799583333333334</v>
+        <v>0.07125000000000004</v>
       </c>
       <c r="C9">
-        <v>0.0625635947731098</v>
+        <v>0.0580678103358423</v>
       </c>
       <c r="D9">
-        <v>266.3021354513329</v>
+        <v>266.4207555943716</v>
       </c>
       <c r="E9">
-        <v>0.02992457402147114</v>
+        <v>0.03046026007377527</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2">
-        <v>34128</v>
+        <v>34155.25</v>
       </c>
       <c r="B10">
-        <v>0.08041666666666673</v>
+        <v>0.07162500000000004</v>
       </c>
       <c r="C10">
-        <v>0.06381908343450959</v>
+        <v>0.0580331255961255</v>
       </c>
       <c r="D10">
-        <v>266.364699046106</v>
+        <v>266.4788234047074</v>
       </c>
       <c r="E10">
-        <v>0.03020710988969238</v>
+        <v>0.03072249307474716</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2">
-        <v>34158</v>
+        <v>34185.66666666666</v>
       </c>
       <c r="B11">
-        <v>0.08087500000000007</v>
+        <v>0.07200000000000004</v>
       </c>
       <c r="C11">
-        <v>0.06237283884081535</v>
+        <v>0.05126530838526833</v>
       </c>
       <c r="D11">
-        <v>266.4285181295405</v>
+        <v>266.5368565303036</v>
       </c>
       <c r="E11">
-        <v>0.03049531551810367</v>
+        <v>0.03098456944016951</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2">
-        <v>34189</v>
+        <v>34246.5</v>
       </c>
       <c r="B12">
-        <v>0.08133333333333341</v>
+        <v>0.07237500000000004</v>
       </c>
       <c r="C12">
-        <v>0.06037323245743664</v>
+        <v>1.4327602802191</v>
       </c>
       <c r="D12">
-        <v>266.4908909683813</v>
+        <v>264.6498363187023</v>
       </c>
       <c r="E12">
-        <v>0.03077698993657692</v>
+        <v>0.02246282615209299</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2">
-        <v>34250</v>
+        <v>34276.91666666666</v>
       </c>
       <c r="B13">
-        <v>0.08179166666666675</v>
+        <v>0.07275000000000004</v>
       </c>
       <c r="C13">
-        <v>1.420046854699649</v>
+        <v>0.459227163816422</v>
       </c>
       <c r="D13">
-        <v>264.6343813427967</v>
+        <v>266.0825965989214</v>
       </c>
       <c r="E13">
-        <v>0.02239303180840676</v>
+        <v>0.02893314121619038</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2">
-        <v>34281</v>
+        <v>34307.33333333334</v>
       </c>
       <c r="B14">
-        <v>0.08225000000000009</v>
+        <v>0.07312500000000004</v>
       </c>
       <c r="C14">
-        <v>0.4621463878258965</v>
+        <v>0.1777252904853412</v>
       </c>
       <c r="D14">
-        <v>266.0544281974963</v>
+        <v>266.5418237627379</v>
       </c>
       <c r="E14">
-        <v>0.0288059333122664</v>
+        <v>0.03100700135658308</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2">
-        <v>34311</v>
+        <v>34337.75</v>
       </c>
       <c r="B15">
-        <v>0.08270833333333343</v>
+        <v>0.07350000000000004</v>
       </c>
       <c r="C15">
-        <v>0.1823576445233357</v>
+        <v>0.09727792999956364</v>
       </c>
       <c r="D15">
-        <v>266.5165745853222</v>
+        <v>266.7195490532232</v>
       </c>
       <c r="E15">
-        <v>0.03089297660642508</v>
+        <v>0.03180960500226925</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2">
-        <v>34342</v>
+        <v>34368.16666666666</v>
       </c>
       <c r="B16">
-        <v>0.08316666666666676</v>
+        <v>0.07387500000000004</v>
       </c>
       <c r="C16">
-        <v>0.097640226465046</v>
+        <v>0.06889658017303191</v>
       </c>
       <c r="D16">
-        <v>266.6989322298456</v>
+        <v>266.8168269832228</v>
       </c>
       <c r="E16">
-        <v>0.03171649986478355</v>
+        <v>0.03224891007274776</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <v>34373</v>
+        <v>34398.58333333334</v>
       </c>
       <c r="B17">
-        <v>0.0836250000000001</v>
+        <v>0.07425000000000004</v>
       </c>
       <c r="C17">
-        <v>0.07349657719623792</v>
+        <v>0.05448559337821735</v>
       </c>
       <c r="D17">
-        <v>266.7965724563106</v>
+        <v>266.8857235633958</v>
       </c>
       <c r="E17">
-        <v>0.03215744105842271</v>
+        <v>0.03256004556883393</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2">
-        <v>34401</v>
+        <v>34459.41666666666</v>
       </c>
       <c r="B18">
-        <v>0.08408333333333344</v>
+        <v>0.07462500000000004</v>
       </c>
       <c r="C18">
-        <v>0.05773164433139755</v>
+        <v>1.51012814240562</v>
       </c>
       <c r="D18">
-        <v>266.8700690335069</v>
+        <v>264.8647193946255</v>
       </c>
       <c r="E18">
-        <v>0.03248935004358773</v>
+        <v>0.02343323356941231</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2">
-        <v>34462</v>
+        <v>34489.83333333334</v>
       </c>
       <c r="B19">
-        <v>0.08454166666666678</v>
+        <v>0.07500000000000004</v>
       </c>
       <c r="C19">
-        <v>1.514922712840757</v>
+        <v>0.4954357650026395</v>
       </c>
       <c r="D19">
-        <v>264.8708796902342</v>
+        <v>266.3748475370311</v>
       </c>
       <c r="E19">
-        <v>0.02346105333383965</v>
+        <v>0.03025294025965507</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2">
-        <v>34493</v>
+        <v>34520.25</v>
       </c>
       <c r="B20">
-        <v>0.08500000000000012</v>
+        <v>0.07537500000000004</v>
       </c>
       <c r="C20">
-        <v>0.5023662713640533</v>
+        <v>0.1933605418848856</v>
       </c>
       <c r="D20">
-        <v>266.385802403075</v>
+        <v>266.8702833020337</v>
       </c>
       <c r="E20">
-        <v>0.03030241220256687</v>
+        <v>0.03249031767571452</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2">
-        <v>34523</v>
+        <v>34550.66666666666</v>
       </c>
       <c r="B21">
-        <v>0.08545833333333346</v>
+        <v>0.07575000000000004</v>
       </c>
       <c r="C21">
-        <v>0.1905333846599433</v>
+        <v>0.101882365768688</v>
       </c>
       <c r="D21">
-        <v>266.888168674439</v>
+        <v>267.0636438439186</v>
       </c>
       <c r="E21">
-        <v>0.03257108763849122</v>
+        <v>0.03336352978539744</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2">
-        <v>34554</v>
+        <v>34581.08333333334</v>
       </c>
       <c r="B22">
-        <v>0.08591666666666679</v>
+        <v>0.07612500000000004</v>
       </c>
       <c r="C22">
-        <v>0.1059323666178216</v>
+        <v>0.07165648415548276</v>
       </c>
       <c r="D22">
-        <v>267.078702059099</v>
+        <v>267.1655262096873</v>
       </c>
       <c r="E22">
-        <v>0.03343153236605604</v>
+        <v>0.03382362839023733</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2">
-        <v>34585</v>
+        <v>34611.5</v>
       </c>
       <c r="B23">
-        <v>0.08637500000000013</v>
+        <v>0.07650000000000004</v>
       </c>
       <c r="C23">
-        <v>0.07602074457952313</v>
+        <v>0.06170404484350911</v>
       </c>
       <c r="D23">
-        <v>267.1846344257168</v>
+        <v>267.2371826938428</v>
       </c>
       <c r="E23">
-        <v>0.0339099206889079</v>
+        <v>0.03414722755422357</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2">
-        <v>34615</v>
+        <v>34641.91666666666</v>
       </c>
       <c r="B24">
-        <v>0.08683333333333347</v>
+        <v>0.07687500000000004</v>
       </c>
       <c r="C24">
-        <v>0.06872656558152812</v>
+        <v>0.05746045110686282</v>
       </c>
       <c r="D24">
-        <v>267.2606551702963</v>
+        <v>267.2988867386863</v>
       </c>
       <c r="E24">
-        <v>0.03425322876048664</v>
+        <v>0.0344258817131773</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2">
-        <v>34646</v>
+        <v>34672.33333333334</v>
       </c>
       <c r="B25">
-        <v>0.08729166666666681</v>
+        <v>0.07725000000000004</v>
       </c>
       <c r="C25">
-        <v>0.06594036907756617</v>
+        <v>0.05720748166913836</v>
       </c>
       <c r="D25">
-        <v>267.3293817358779</v>
+        <v>267.3563471897932</v>
       </c>
       <c r="E25">
-        <v>0.0345635964742803</v>
+        <v>0.03468537189274141</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2">
-        <v>34676</v>
+        <v>34702.75</v>
       </c>
       <c r="B26">
-        <v>0.08775000000000015</v>
+        <v>0.07762500000000004</v>
       </c>
       <c r="C26">
-        <v>0.06692460829526681</v>
+        <v>0.05818537288723746</v>
       </c>
       <c r="D26">
-        <v>267.3953221049554</v>
+        <v>267.4135546714623</v>
       </c>
       <c r="E26">
-        <v>0.03486138178370374</v>
+        <v>0.03494371966768552</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2">
-        <v>34707</v>
+        <v>34733.16666666666</v>
       </c>
       <c r="B27">
-        <v>0.08820833333333349</v>
+        <v>0.07800000000000004</v>
       </c>
       <c r="C27">
-        <v>0.06504760988150338</v>
+        <v>0.05886904613839761</v>
       </c>
       <c r="D27">
-        <v>267.4622467132507</v>
+        <v>267.4717400443495</v>
       </c>
       <c r="E27">
-        <v>0.03516361189657741</v>
+        <v>0.0352064835786483</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2">
-        <v>34738</v>
+        <v>34763.58333333334</v>
       </c>
       <c r="B28">
-        <v>0.08866666666666682</v>
+        <v>0.07837500000000004</v>
       </c>
       <c r="C28">
-        <v>0.0650615027875574</v>
+        <v>0.06012537664742013</v>
       </c>
       <c r="D28">
-        <v>267.5272943231322</v>
+        <v>267.5306090904879</v>
       </c>
       <c r="E28">
-        <v>0.03545736552438983</v>
+        <v>0.0354723349435257</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2">
-        <v>34766</v>
+        <v>34794</v>
       </c>
       <c r="B29">
-        <v>0.08912500000000016</v>
+        <v>0.07875000000000004</v>
       </c>
       <c r="C29">
-        <v>0.06508971954326626</v>
+        <v>-0.9833062563091062</v>
       </c>
       <c r="D29">
-        <v>267.5923558259198</v>
+        <v>267.5907344671353</v>
       </c>
       <c r="E29">
-        <v>0.03575118189227154</v>
+        <v>0.03574385987035922</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2">
-        <v>34797</v>
+        <v>34824.41666666666</v>
       </c>
       <c r="B30">
-        <v>0.0895833333333335</v>
+        <v>0</v>
       </c>
       <c r="C30">
+        <v>-3.145413614594418</v>
+      </c>
+      <c r="D30">
+        <v>266.6074282108262</v>
+      </c>
+      <c r="E30">
+        <v>0.03130326965393775</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>34854.83333333334</v>
+      </c>
+      <c r="B31">
         <v>0</v>
       </c>
-      <c r="D30">
-        <v>267.657445545463</v>
-      </c>
-      <c r="E30">
-        <v>0.03604512568642405</v>
+      <c r="C31">
+        <v>-0.765263432317056</v>
+      </c>
+      <c r="D31">
+        <v>263.4620145962318</v>
+      </c>
+      <c r="E31">
+        <v>0.01709864842433816</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>34885.25</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>-0.1810545362226321</v>
+      </c>
+      <c r="D32">
+        <v>262.6967511639148</v>
+      </c>
+      <c r="E32">
+        <v>0.0136427349805576</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2">
+        <v>34915.66666666666</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>-0.04382037918185233</v>
+      </c>
+      <c r="D33">
+        <v>262.5156966276921</v>
+      </c>
+      <c r="E33">
+        <v>0.01282509653167121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2">
+        <v>34946.08333333334</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>-0.01029744913398645</v>
+      </c>
+      <c r="D34">
+        <v>262.4718762485103</v>
+      </c>
+      <c r="E34">
+        <v>0.01262720462787591</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2">
+        <v>34976.5</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>-0.002418845670035807</v>
+      </c>
+      <c r="D35">
+        <v>262.4615787993763</v>
+      </c>
+      <c r="E35">
+        <v>0.01258070156579822</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2">
+        <v>35006.91666666666</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>-0.0005681271595676662</v>
+      </c>
+      <c r="D36">
+        <v>262.4591599537063</v>
+      </c>
+      <c r="E36">
+        <v>0.01256977811000981</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2">
+        <v>35037.33333333334</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>-0.2423775537899928</v>
+      </c>
+      <c r="D37">
+        <v>262.4585918265467</v>
+      </c>
+      <c r="E37">
+        <v>0.01256721245979624</v>
       </c>
     </row>
   </sheetData>
@@ -2679,7 +2798,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2708,6 +2827,312 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>35098.16666666666</v>
+      </c>
+      <c r="B2">
+        <v>0.03004166666666666</v>
+      </c>
+      <c r="C2">
+        <v>1.255940521069761</v>
+      </c>
+      <c r="D2">
+        <v>263.7003188540895</v>
+      </c>
+      <c r="E2">
+        <v>0.01741321572615493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>35128.58333333334</v>
+      </c>
+      <c r="B3">
+        <v>0.03008333333333333</v>
+      </c>
+      <c r="C3">
+        <v>0.3591437145022383</v>
+      </c>
+      <c r="D3">
+        <v>264.9562593751592</v>
+      </c>
+      <c r="E3">
+        <v>0.02305734432069878</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>35159</v>
+      </c>
+      <c r="B4">
+        <v>0.030125</v>
+      </c>
+      <c r="C4">
+        <v>0.1208166117150995</v>
+      </c>
+      <c r="D4">
+        <v>265.3154030896615</v>
+      </c>
+      <c r="E4">
+        <v>0.02465801131399439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
+        <v>35189.41666666666</v>
+      </c>
+      <c r="B5">
+        <v>0.03016666666666666</v>
+      </c>
+      <c r="C5">
+        <v>0.07152286182179068</v>
+      </c>
+      <c r="D5">
+        <v>265.4362197013766</v>
+      </c>
+      <c r="E5">
+        <v>0.02540103015136833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>35219.83333333334</v>
+      </c>
+      <c r="B6">
+        <v>0.03020833333333333</v>
+      </c>
+      <c r="C6">
+        <v>0.0552045208518166</v>
+      </c>
+      <c r="D6">
+        <v>265.5077425631983</v>
+      </c>
+      <c r="E6">
+        <v>0.0258567955966334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>35250.25</v>
+      </c>
+      <c r="B7">
+        <v>0.03024999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.06103690015595475</v>
+      </c>
+      <c r="D7">
+        <v>265.5629470840502</v>
+      </c>
+      <c r="E7">
+        <v>0.02639379685562324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>35280.66666666666</v>
+      </c>
+      <c r="B8">
+        <v>0.03029166666666666</v>
+      </c>
+      <c r="C8">
+        <v>0.03285404319944973</v>
+      </c>
+      <c r="D8">
+        <v>265.6239839842061</v>
+      </c>
+      <c r="E8">
+        <v>0.02666943820330527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>35402.33333333334</v>
+      </c>
+      <c r="B9">
+        <v>0.03037499999999999</v>
+      </c>
+      <c r="C9">
+        <v>1.066764461531534</v>
+      </c>
+      <c r="D9">
+        <v>264.2075302762878</v>
+      </c>
+      <c r="E9">
+        <v>0.01915758983574864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>35554.41666666666</v>
+      </c>
+      <c r="B10">
+        <v>0.03508333333333334</v>
+      </c>
+      <c r="C10">
+        <v>1.173806863841946</v>
+      </c>
+      <c r="D10">
+        <v>264.3994826637073</v>
+      </c>
+      <c r="E10">
+        <v>0.02069949550783361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>35615.25</v>
+      </c>
+      <c r="B11">
+        <v>0.03512500000000001</v>
+      </c>
+      <c r="C11">
+        <v>1.044887893699524</v>
+      </c>
+      <c r="D11">
+        <v>264.424734142607</v>
+      </c>
+      <c r="E11">
+        <v>0.01834844082933927</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>35645.66666666666</v>
+      </c>
+      <c r="B12">
+        <v>0.03516666666666668</v>
+      </c>
+      <c r="C12">
+        <v>0.4255370755721515</v>
+      </c>
+      <c r="D12">
+        <v>265.4696220363065</v>
+      </c>
+      <c r="E12">
+        <v>0.02495939040138997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>35676.08333333334</v>
+      </c>
+      <c r="B13">
+        <v>0.03520833333333335</v>
+      </c>
+      <c r="C13">
+        <v>0.09829939176313474</v>
+      </c>
+      <c r="D13">
+        <v>265.8951591118787</v>
+      </c>
+      <c r="E13">
+        <v>0.02622029368308197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>35706.5</v>
+      </c>
+      <c r="B14">
+        <v>0.03525000000000002</v>
+      </c>
+      <c r="C14">
+        <v>0.06453921984643785</v>
+      </c>
+      <c r="D14">
+        <v>265.9934585036418</v>
+      </c>
+      <c r="E14">
+        <v>0.02687929058963887</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>35858.58333333334</v>
+      </c>
+      <c r="B15">
+        <v>0.03529166666666669</v>
+      </c>
+      <c r="C15">
+        <v>0.8549868071165747</v>
+      </c>
+      <c r="D15">
+        <v>264.5279993593723</v>
+      </c>
+      <c r="E15">
+        <v>0.01499937102718732</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>35889</v>
+      </c>
+      <c r="B16">
+        <v>0.03533333333333336</v>
+      </c>
+      <c r="C16">
+        <v>0.4284030774456369</v>
+      </c>
+      <c r="D16">
+        <v>265.3829861664889</v>
+      </c>
+      <c r="E16">
+        <v>0.02176372498485314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>36010.66666666666</v>
+      </c>
+      <c r="B17">
+        <v>0.03537500000000002</v>
+      </c>
+      <c r="C17">
+        <v>1.029639039197377</v>
+      </c>
+      <c r="D17">
+        <v>264.5812448071053</v>
+      </c>
+      <c r="E17">
+        <v>0.01783679037263674</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>36041.08333333334</v>
+      </c>
+      <c r="B18">
+        <v>0.03541666666666669</v>
+      </c>
+      <c r="C18">
+        <v>0.3096733910042531</v>
+      </c>
+      <c r="D18">
+        <v>265.6108838463027</v>
+      </c>
+      <c r="E18">
+        <v>0.02243366008748182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>36071.5</v>
+      </c>
+      <c r="B19">
+        <v>0.03545833333333336</v>
+      </c>
+      <c r="C19">
+        <v>-0.01628359478741004</v>
+      </c>
+      <c r="D19">
+        <v>265.920557237307</v>
+      </c>
+      <c r="E19">
+        <v>0.02173288729125258</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2715,7 +3140,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2742,6 +3167,312 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>36132.33333333334</v>
+      </c>
+      <c r="B2">
+        <v>0.0355416666666667</v>
+      </c>
+      <c r="C2">
+        <v>-0.5612555084132964</v>
+      </c>
+      <c r="D2">
+        <v>264.6106940592622</v>
+      </c>
+      <c r="E2">
+        <v>0.02084491309915609</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>36162.75</v>
+      </c>
+      <c r="B3">
+        <v>0.03558333333333337</v>
+      </c>
+      <c r="C3">
+        <v>-0.3773302507239578</v>
+      </c>
+      <c r="D3">
+        <v>264.0494385508489</v>
+      </c>
+      <c r="E3">
+        <v>0.01401087958013952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>36193.16666666666</v>
+      </c>
+      <c r="B4">
+        <v>0.03562500000000004</v>
+      </c>
+      <c r="C4">
+        <v>-0.1275478447419118</v>
+      </c>
+      <c r="D4">
+        <v>263.6721083001249</v>
+      </c>
+      <c r="E4">
+        <v>0.01135767178455273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
+        <v>36223.58333333334</v>
+      </c>
+      <c r="B5">
+        <v>0.03566666666666671</v>
+      </c>
+      <c r="C5">
+        <v>-0.085885347400108</v>
+      </c>
+      <c r="D5">
+        <v>263.544560455383</v>
+      </c>
+      <c r="E5">
+        <v>0.009450130278141435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>36254</v>
+      </c>
+      <c r="B6">
+        <v>0.03570833333333338</v>
+      </c>
+      <c r="C6">
+        <v>0.002090258361249653</v>
+      </c>
+      <c r="D6">
+        <v>263.4586751079829</v>
+      </c>
+      <c r="E6">
+        <v>0.009151552268151565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>36375.66666666666</v>
+      </c>
+      <c r="B7">
+        <v>0.03575000000000005</v>
+      </c>
+      <c r="C7">
+        <v>0.3738162672055978</v>
+      </c>
+      <c r="D7">
+        <v>262.9715959368194</v>
+      </c>
+      <c r="E7">
+        <v>0.006468004682852053</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>36406.08333333334</v>
+      </c>
+      <c r="B8">
+        <v>0.03579166666666671</v>
+      </c>
+      <c r="C8">
+        <v>0.1126154424498509</v>
+      </c>
+      <c r="D8">
+        <v>263.345412204025</v>
+      </c>
+      <c r="E8">
+        <v>0.008045923491922399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>36436.5</v>
+      </c>
+      <c r="B9">
+        <v>0.03583333333333338</v>
+      </c>
+      <c r="C9">
+        <v>0.03467454698659367</v>
+      </c>
+      <c r="D9">
+        <v>263.4580276464749</v>
+      </c>
+      <c r="E9">
+        <v>0.008184350040406527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>36466.91666666666</v>
+      </c>
+      <c r="B10">
+        <v>0.03587500000000005</v>
+      </c>
+      <c r="C10">
+        <v>-0.1045023356716683</v>
+      </c>
+      <c r="D10">
+        <v>263.4927021934615</v>
+      </c>
+      <c r="E10">
+        <v>0.005773056095632657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>36497.33333333334</v>
+      </c>
+      <c r="B11">
+        <v>0.03591666666666672</v>
+      </c>
+      <c r="C11">
+        <v>-0.003164701325204078</v>
+      </c>
+      <c r="D11">
+        <v>263.3881998577898</v>
+      </c>
+      <c r="E11">
+        <v>0.005248829015242937</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>36527.75</v>
+      </c>
+      <c r="B12">
+        <v>0.03595833333333339</v>
+      </c>
+      <c r="C12">
+        <v>0.04523454233526536</v>
+      </c>
+      <c r="D12">
+        <v>263.3850351564646</v>
+      </c>
+      <c r="E12">
+        <v>0.005605996260530096</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>36558.16666666666</v>
+      </c>
+      <c r="B13">
+        <v>0.03600000000000006</v>
+      </c>
+      <c r="C13">
+        <v>-0.04655679195059292</v>
+      </c>
+      <c r="D13">
+        <v>263.4302696987999</v>
+      </c>
+      <c r="E13">
+        <v>0.004334714293482152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>36619</v>
+      </c>
+      <c r="B14">
+        <v>0.0360833333333334</v>
+      </c>
+      <c r="C14">
+        <v>0.1622299500941153</v>
+      </c>
+      <c r="D14">
+        <v>263.1729738080409</v>
+      </c>
+      <c r="E14">
+        <v>0.002504541751184976</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>36649.41666666666</v>
+      </c>
+      <c r="B15">
+        <v>0.03612500000000007</v>
+      </c>
+      <c r="C15">
+        <v>0.05613848489360862</v>
+      </c>
+      <c r="D15">
+        <v>263.335203758135</v>
+      </c>
+      <c r="E15">
+        <v>0.003095187455210728</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>36679.83333333334</v>
+      </c>
+      <c r="B16">
+        <v>0.03616666666666674</v>
+      </c>
+      <c r="C16">
+        <v>0.04402037918680435</v>
+      </c>
+      <c r="D16">
+        <v>263.3913422430286</v>
+      </c>
+      <c r="E16">
+        <v>0.003471214302327701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>36710.25</v>
+      </c>
+      <c r="B17">
+        <v>0.0362083333333334</v>
+      </c>
+      <c r="C17">
+        <v>0.001834113729046294</v>
+      </c>
+      <c r="D17">
+        <v>263.4353626222154</v>
+      </c>
+      <c r="E17">
+        <v>0.00313726967971246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>36892.75</v>
+      </c>
+      <c r="B18">
+        <v>0.03629166666666674</v>
+      </c>
+      <c r="C18">
+        <v>0.4594225343930702</v>
+      </c>
+      <c r="D18">
+        <v>263.2938306262027</v>
+      </c>
+      <c r="E18">
+        <v>0.007842672215247991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>36923.16666666666</v>
+      </c>
+      <c r="B19">
+        <v>0.03633333333333341</v>
+      </c>
+      <c r="C19">
+        <v>0.206015046612265</v>
+      </c>
+      <c r="D19">
+        <v>263.7532531605958</v>
+      </c>
+      <c r="E19">
+        <v>0.0109340374746827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
underprediction in phase 3
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -7,27 +7,28 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Phase 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Phase 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Phase 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Phase 5_6" sheetId="5" r:id="rId5"/>
-    <sheet name="Phase 7" sheetId="6" r:id="rId6"/>
+    <sheet name="Phase 1 Pre CPP" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase 1 Post CPP" sheetId="2" r:id="rId2"/>
+    <sheet name="Phase 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Phase 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Phase 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Phase 5_6" sheetId="6" r:id="rId6"/>
+    <sheet name="Phase 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
   <si>
     <t>DP leakage</t>
   </si>
   <si>
-    <t>Delta RIHT_2</t>
+    <t>Delta RIHT</t>
   </si>
   <si>
-    <t>RIHT_2</t>
+    <t>RIHT</t>
   </si>
   <si>
     <t>Steam quality</t>
@@ -576,6 +577,48 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
fast mode wasnt treating tubes that didn't refurb vs both cleanings vs just one of right
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -41,6 +41,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -93,9 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -392,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,6 +425,23 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>30414</v>
+      </c>
+      <c r="B2">
+        <v>0.03033333333333333</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>261.8439554330322</v>
+      </c>
+      <c r="E2">
+        <v>0.009791527531336826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
purification not working well...concentration runaway
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8427607064544</v>
+        <v>261.842803894764</v>
       </c>
       <c r="F2">
-        <v>0.007478727091303701</v>
+        <v>0.007478922128794388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed runaway concentration...timestep hardcoded as 1 mo into sludge and divider plate functions
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -437,7 +437,7 @@
         <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.03033333333333333</v>
+        <v>0.03000045662100457</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.842803894764</v>
+        <v>261.8006959847297</v>
       </c>
       <c r="F2">
-        <v>0.007478922128794388</v>
+        <v>0.007288763699380986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
timestep errors fixed n div plate and sludge fuling functions
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -437,7 +437,7 @@
         <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.03000045662100457</v>
+        <v>0.03</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8006959847297</v>
+        <v>261.8012363150606</v>
       </c>
       <c r="F2">
-        <v>0.007288763699380986</v>
+        <v>0.00729120381970518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing oxide growth and reduction from refurb
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -437,7 +437,7 @@
         <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.03000456621004566</v>
+        <v>0.03041666666666666</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8028894482187</v>
+        <v>261.8820422433974</v>
       </c>
       <c r="F2">
-        <v>0.007298669334016065</v>
+        <v>0.007656121679730205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ox thickness reduction not working
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8820422433974</v>
+        <v>261.8831256424503</v>
       </c>
       <c r="F2">
-        <v>0.007656121679730205</v>
+        <v>0.007661014286894672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
took all selected tubes stuff out...all bundles run now
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8831256424503</v>
+        <v>261.8815758431489</v>
       </c>
       <c r="F2">
-        <v>0.007661014286894672</v>
+        <v>0.007654015426091007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error in preheater calc
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -437,7 +437,7 @@
         <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.03041666666666666</v>
+        <v>0.03</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8815758431489</v>
+        <v>261.8784580676896</v>
       </c>
       <c r="F2">
-        <v>0.007654015426091007</v>
+        <v>0.007639935618185261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slope still too high post CPP
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8479215206169</v>
+        <v>261.8323033063213</v>
       </c>
       <c r="F2">
-        <v>0.01094129071127611</v>
+        <v>0.01087100359612432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resistances for oxide layers can't be changed.
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2040786</v>
       </c>
       <c r="E2">
-        <v>261.8323033063213</v>
+        <v>261.9205476730947</v>
       </c>
       <c r="F2">
-        <v>0.01087100359612432</v>
+        <v>0.01126813234922662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error in spalling carrying through to SG - still not quite right
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -434,162 +434,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>30477</v>
+        <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.06046027416438356</v>
+        <v>0.035</v>
       </c>
       <c r="C2">
-        <v>0.2297240643719078</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>262.3108460275721</v>
+        <v>260.8258482527681</v>
       </c>
       <c r="F2">
-        <v>0.0153240129987072</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2">
-        <v>30484</v>
-      </c>
-      <c r="B3">
-        <v>0.06049863032876712</v>
-      </c>
-      <c r="C3">
-        <v>0.05912997657048891</v>
-      </c>
-      <c r="D3">
-        <v>2061400</v>
-      </c>
-      <c r="E3">
-        <v>262.540570091944</v>
-      </c>
-      <c r="F3">
-        <v>0.01635784705041258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2">
-        <v>30491</v>
-      </c>
-      <c r="B4">
-        <v>0.06053698649315067</v>
-      </c>
-      <c r="C4">
-        <v>0.02178056795116845</v>
-      </c>
-      <c r="D4">
-        <v>2061400</v>
-      </c>
-      <c r="E4">
-        <v>262.5997000685145</v>
-      </c>
-      <c r="F4">
-        <v>0.01662395144579781</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2">
-        <v>30498</v>
-      </c>
-      <c r="B5">
-        <v>0.06057534265753423</v>
-      </c>
-      <c r="C5">
-        <v>0.01298175072281538</v>
-      </c>
-      <c r="D5">
-        <v>2061400</v>
-      </c>
-      <c r="E5">
-        <v>262.6214806364657</v>
-      </c>
-      <c r="F5">
-        <v>0.01672197118471806</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2">
-        <v>30505</v>
-      </c>
-      <c r="B6">
-        <v>0.06061369882191779</v>
-      </c>
-      <c r="C6">
-        <v>0.01041546893441136</v>
-      </c>
-      <c r="D6">
-        <v>2061400</v>
-      </c>
-      <c r="E6">
-        <v>262.6344623871885</v>
-      </c>
-      <c r="F6">
-        <v>0.01678039334429761</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2">
-        <v>30512</v>
-      </c>
-      <c r="B7">
-        <v>0.06065205498630135</v>
-      </c>
-      <c r="C7">
-        <v>0.009261817087804047</v>
-      </c>
-      <c r="D7">
-        <v>2061400</v>
-      </c>
-      <c r="E7">
-        <v>262.6448778561229</v>
-      </c>
-      <c r="F7">
-        <v>0.0168272663894802</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>30519</v>
-      </c>
-      <c r="B8">
-        <v>0.06069041115068491</v>
-      </c>
-      <c r="C8">
-        <v>0.008743877345182227</v>
-      </c>
-      <c r="D8">
-        <v>2061400</v>
-      </c>
-      <c r="E8">
-        <v>262.6541396732107</v>
-      </c>
-      <c r="F8">
-        <v>0.01686894762088384</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>30526</v>
-      </c>
-      <c r="B9">
-        <v>0.06072876731506847</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>2061400</v>
-      </c>
-      <c r="E9">
-        <v>262.6628835505559</v>
-      </c>
-      <c r="F9">
-        <v>0.01690829795263113</v>
+        <v>0.008641033266058135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made concentration output as input into next run
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>260.8258482527681</v>
+        <v>261.7662441132131</v>
       </c>
       <c r="F2">
-        <v>0.008641033266058135</v>
+        <v>0.01287312477666711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bundle sizes need to be saved and used as future input as well
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>261.7662441132131</v>
+        <v>261.7651854938841</v>
       </c>
       <c r="F2">
-        <v>0.01287312477666711</v>
+        <v>0.01286836064055835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bundle size input and cleaned up cleaning functions
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>261.7651854938841</v>
+        <v>262.6355143976893</v>
       </c>
       <c r="F2">
-        <v>0.01286836064055835</v>
+        <v>0.01678512773850001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
outages stopped working - testing fix
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>262.6355143976893</v>
+        <v>262.6354771454063</v>
       </c>
       <c r="F2">
-        <v>0.01678512773850001</v>
+        <v>0.01678496009094076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sorted ox growth post run end
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -446,10 +446,10 @@
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>262.6354771454063</v>
+        <v>262.6353826259896</v>
       </c>
       <c r="F2">
-        <v>0.01678496009094076</v>
+        <v>0.01678453472239336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temp. dependence on kp needed to be uped (flat lines deposit at lower val. for colder temps)
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,6 +430,266 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2">
+        <v>30414</v>
+      </c>
+      <c r="B2">
+        <v>0.03507671232876713</v>
+      </c>
+      <c r="C2">
+        <v>0.09775300847218205</v>
+      </c>
+      <c r="D2">
+        <v>2061400</v>
+      </c>
+      <c r="E2">
+        <v>261.6055012161822</v>
+      </c>
+      <c r="F2">
+        <v>0.01214972872769548</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>30421</v>
+      </c>
+      <c r="B3">
+        <v>0.03515342465753425</v>
+      </c>
+      <c r="C3">
+        <v>0.02691860832419479</v>
+      </c>
+      <c r="D3">
+        <v>2061400</v>
+      </c>
+      <c r="E3">
+        <v>261.7032542246544</v>
+      </c>
+      <c r="F3">
+        <v>0.01258964950435209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>30428</v>
+      </c>
+      <c r="B4">
+        <v>0.03523013698630138</v>
+      </c>
+      <c r="C4">
+        <v>0.01348364722775841</v>
+      </c>
+      <c r="D4">
+        <v>2061400</v>
+      </c>
+      <c r="E4">
+        <v>261.7301728329786</v>
+      </c>
+      <c r="F4">
+        <v>0.01271079211945501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>30435</v>
+      </c>
+      <c r="B5">
+        <v>0.0353068493150685</v>
+      </c>
+      <c r="C5">
+        <v>0.01006806763882651</v>
+      </c>
+      <c r="D5">
+        <v>2061400</v>
+      </c>
+      <c r="E5">
+        <v>261.7436564802064</v>
+      </c>
+      <c r="F5">
+        <v>0.01277147297883006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>30442</v>
+      </c>
+      <c r="B6">
+        <v>0.03538356164383562</v>
+      </c>
+      <c r="C6">
+        <v>0.005773520527213805</v>
+      </c>
+      <c r="D6">
+        <v>2061400</v>
+      </c>
+      <c r="E6">
+        <v>261.7537245478452</v>
+      </c>
+      <c r="F6">
+        <v>0.01281678260361123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>30477</v>
+      </c>
+      <c r="B7">
+        <v>0.05007671232876713</v>
+      </c>
+      <c r="C7">
+        <v>0.5486457479805722</v>
+      </c>
+      <c r="D7">
+        <v>2061400</v>
+      </c>
+      <c r="E7">
+        <v>261.7772524173773</v>
+      </c>
+      <c r="F7">
+        <v>0.01292266577589849</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>30484</v>
+      </c>
+      <c r="B8">
+        <v>0.05015342465753425</v>
+      </c>
+      <c r="C8">
+        <v>0.1177744491453723</v>
+      </c>
+      <c r="D8">
+        <v>2061400</v>
+      </c>
+      <c r="E8">
+        <v>262.3258981653579</v>
+      </c>
+      <c r="F8">
+        <v>0.01539175258287509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>30491</v>
+      </c>
+      <c r="B9">
+        <v>0.05023013698630138</v>
+      </c>
+      <c r="C9">
+        <v>0.03045935413138068</v>
+      </c>
+      <c r="D9">
+        <v>2061400</v>
+      </c>
+      <c r="E9">
+        <v>262.4436726145033</v>
+      </c>
+      <c r="F9">
+        <v>0.01592177644554819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>30498</v>
+      </c>
+      <c r="B10">
+        <v>0.0503068493150685</v>
+      </c>
+      <c r="C10">
+        <v>0.01318822766370431</v>
+      </c>
+      <c r="D10">
+        <v>2061400</v>
+      </c>
+      <c r="E10">
+        <v>262.4741319686347</v>
+      </c>
+      <c r="F10">
+        <v>0.01605885358450647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>30505</v>
+      </c>
+      <c r="B11">
+        <v>0.05038356164383562</v>
+      </c>
+      <c r="C11">
+        <v>0.01121036431754874</v>
+      </c>
+      <c r="D11">
+        <v>2061400</v>
+      </c>
+      <c r="E11">
+        <v>262.4873201962984</v>
+      </c>
+      <c r="F11">
+        <v>0.01611820495841521</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>30512</v>
+      </c>
+      <c r="B12">
+        <v>0.05046027397260275</v>
+      </c>
+      <c r="C12">
+        <v>0.01019256660379142</v>
+      </c>
+      <c r="D12">
+        <v>2061400</v>
+      </c>
+      <c r="E12">
+        <v>262.4985305606159</v>
+      </c>
+      <c r="F12">
+        <v>0.01616865529497527</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>30519</v>
+      </c>
+      <c r="B13">
+        <v>0.05053698630136987</v>
+      </c>
+      <c r="C13">
+        <v>0.01017217838966644</v>
+      </c>
+      <c r="D13">
+        <v>2061400</v>
+      </c>
+      <c r="E13">
+        <v>262.5087231272197</v>
+      </c>
+      <c r="F13">
+        <v>0.01621452520615798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>30526</v>
+      </c>
+      <c r="B14">
+        <v>0.050613698630137</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2061400</v>
+      </c>
+      <c r="E14">
+        <v>262.5188953056094</v>
+      </c>
+      <c r="F14">
+        <v>0.01626030336365317</v>
       </c>
     </row>
   </sheetData>
@@ -478,7 +738,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -508,26 +768,6 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2">
-        <v>34796</v>
-      </c>
-      <c r="B2">
-        <v>0.0792164383561659</v>
-      </c>
-      <c r="C2">
-        <v>-1.585119896638389</v>
-      </c>
-      <c r="D2">
-        <v>2061400</v>
-      </c>
-      <c r="E2">
-        <v>267.1615689938457</v>
-      </c>
-      <c r="F2">
-        <v>0.0371538660950056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
still adjusting oxide loading
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,256 +440,16 @@
         <v>0.03507671232876713</v>
       </c>
       <c r="C2">
-        <v>0.09775300847218205</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>2061400</v>
       </c>
       <c r="E2">
-        <v>261.6055012161822</v>
+        <v>261.6063956874585</v>
       </c>
       <c r="F2">
-        <v>0.01214972872769548</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2">
-        <v>30421</v>
-      </c>
-      <c r="B3">
-        <v>0.03515342465753425</v>
-      </c>
-      <c r="C3">
-        <v>0.02691860832419479</v>
-      </c>
-      <c r="D3">
-        <v>2061400</v>
-      </c>
-      <c r="E3">
-        <v>261.7032542246544</v>
-      </c>
-      <c r="F3">
-        <v>0.01258964950435209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2">
-        <v>30428</v>
-      </c>
-      <c r="B4">
-        <v>0.03523013698630138</v>
-      </c>
-      <c r="C4">
-        <v>0.01348364722775841</v>
-      </c>
-      <c r="D4">
-        <v>2061400</v>
-      </c>
-      <c r="E4">
-        <v>261.7301728329786</v>
-      </c>
-      <c r="F4">
-        <v>0.01271079211945501</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2">
-        <v>30435</v>
-      </c>
-      <c r="B5">
-        <v>0.0353068493150685</v>
-      </c>
-      <c r="C5">
-        <v>0.01006806763882651</v>
-      </c>
-      <c r="D5">
-        <v>2061400</v>
-      </c>
-      <c r="E5">
-        <v>261.7436564802064</v>
-      </c>
-      <c r="F5">
-        <v>0.01277147297883006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2">
-        <v>30442</v>
-      </c>
-      <c r="B6">
-        <v>0.03538356164383562</v>
-      </c>
-      <c r="C6">
-        <v>0.005773520527213805</v>
-      </c>
-      <c r="D6">
-        <v>2061400</v>
-      </c>
-      <c r="E6">
-        <v>261.7537245478452</v>
-      </c>
-      <c r="F6">
-        <v>0.01281678260361123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2">
-        <v>30477</v>
-      </c>
-      <c r="B7">
-        <v>0.05007671232876713</v>
-      </c>
-      <c r="C7">
-        <v>0.5486457479805722</v>
-      </c>
-      <c r="D7">
-        <v>2061400</v>
-      </c>
-      <c r="E7">
-        <v>261.7772524173773</v>
-      </c>
-      <c r="F7">
-        <v>0.01292266577589849</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>30484</v>
-      </c>
-      <c r="B8">
-        <v>0.05015342465753425</v>
-      </c>
-      <c r="C8">
-        <v>0.1177744491453723</v>
-      </c>
-      <c r="D8">
-        <v>2061400</v>
-      </c>
-      <c r="E8">
-        <v>262.3258981653579</v>
-      </c>
-      <c r="F8">
-        <v>0.01539175258287509</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>30491</v>
-      </c>
-      <c r="B9">
-        <v>0.05023013698630138</v>
-      </c>
-      <c r="C9">
-        <v>0.03045935413138068</v>
-      </c>
-      <c r="D9">
-        <v>2061400</v>
-      </c>
-      <c r="E9">
-        <v>262.4436726145033</v>
-      </c>
-      <c r="F9">
-        <v>0.01592177644554819</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2">
-        <v>30498</v>
-      </c>
-      <c r="B10">
-        <v>0.0503068493150685</v>
-      </c>
-      <c r="C10">
-        <v>0.01318822766370431</v>
-      </c>
-      <c r="D10">
-        <v>2061400</v>
-      </c>
-      <c r="E10">
-        <v>262.4741319686347</v>
-      </c>
-      <c r="F10">
-        <v>0.01605885358450647</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2">
-        <v>30505</v>
-      </c>
-      <c r="B11">
-        <v>0.05038356164383562</v>
-      </c>
-      <c r="C11">
-        <v>0.01121036431754874</v>
-      </c>
-      <c r="D11">
-        <v>2061400</v>
-      </c>
-      <c r="E11">
-        <v>262.4873201962984</v>
-      </c>
-      <c r="F11">
-        <v>0.01611820495841521</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2">
-        <v>30512</v>
-      </c>
-      <c r="B12">
-        <v>0.05046027397260275</v>
-      </c>
-      <c r="C12">
-        <v>0.01019256660379142</v>
-      </c>
-      <c r="D12">
-        <v>2061400</v>
-      </c>
-      <c r="E12">
-        <v>262.4985305606159</v>
-      </c>
-      <c r="F12">
-        <v>0.01616865529497527</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2">
-        <v>30519</v>
-      </c>
-      <c r="B13">
-        <v>0.05053698630136987</v>
-      </c>
-      <c r="C13">
-        <v>0.01017217838966644</v>
-      </c>
-      <c r="D13">
-        <v>2061400</v>
-      </c>
-      <c r="E13">
-        <v>262.5087231272197</v>
-      </c>
-      <c r="F13">
-        <v>0.01621452520615798</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2">
-        <v>30526</v>
-      </c>
-      <c r="B14">
-        <v>0.050613698630137</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>2061400</v>
-      </c>
-      <c r="E14">
-        <v>262.5188953056094</v>
-      </c>
-      <c r="F14">
-        <v>0.01626030336365317</v>
+        <v>0.01215375414343174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
decreased kd and oxide growth by ~25%
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,19 +437,899 @@
         <v>30414</v>
       </c>
       <c r="B2">
-        <v>0.03507671232876713</v>
+        <v>0.03509589041095891</v>
       </c>
       <c r="C2">
+        <v>0.09859975109270636</v>
+      </c>
+      <c r="D2">
+        <v>2061400</v>
+      </c>
+      <c r="E2">
+        <v>261.6060874113738</v>
+      </c>
+      <c r="F2">
+        <v>0.01215236679938224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>30421</v>
+      </c>
+      <c r="B3">
+        <v>0.03519178082191782</v>
+      </c>
+      <c r="C3">
+        <v>0.02793026466270021</v>
+      </c>
+      <c r="D3">
+        <v>2061400</v>
+      </c>
+      <c r="E3">
+        <v>261.7046871624665</v>
+      </c>
+      <c r="F3">
+        <v>0.01259609819708331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>30428</v>
+      </c>
+      <c r="B4">
+        <v>0.03528767123287672</v>
+      </c>
+      <c r="C4">
+        <v>0.01466782402314948</v>
+      </c>
+      <c r="D4">
+        <v>2061400</v>
+      </c>
+      <c r="E4">
+        <v>261.7326174271292</v>
+      </c>
+      <c r="F4">
+        <v>0.01272179359934941</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>30435</v>
+      </c>
+      <c r="B5">
+        <v>0.03538356164383563</v>
+      </c>
+      <c r="C5">
+        <v>0.01096094085903587</v>
+      </c>
+      <c r="D5">
+        <v>2061400</v>
+      </c>
+      <c r="E5">
+        <v>261.7472852511523</v>
+      </c>
+      <c r="F5">
+        <v>0.01278780364484049</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>30442</v>
+      </c>
+      <c r="B6">
+        <v>0.03547945205479454</v>
+      </c>
+      <c r="C6">
+        <v>0.007776986594194568</v>
+      </c>
+      <c r="D6">
+        <v>2061400</v>
+      </c>
+      <c r="E6">
+        <v>261.7582461920114</v>
+      </c>
+      <c r="F6">
+        <v>0.01283713149357829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>30477</v>
+      </c>
+      <c r="B7">
+        <v>0.05009589041095891</v>
+      </c>
+      <c r="C7">
+        <v>0.5501010033279954</v>
+      </c>
+      <c r="D7">
+        <v>2061400</v>
+      </c>
+      <c r="E7">
+        <v>261.7791361342943</v>
+      </c>
+      <c r="F7">
+        <v>0.01293114312326659</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>30484</v>
+      </c>
+      <c r="B8">
+        <v>0.05019178082191782</v>
+      </c>
+      <c r="C8">
+        <v>0.1194152344637587</v>
+      </c>
+      <c r="D8">
+        <v>2061400</v>
+      </c>
+      <c r="E8">
+        <v>262.3292371376223</v>
+      </c>
+      <c r="F8">
+        <v>0.01540677905924382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>30491</v>
+      </c>
+      <c r="B9">
+        <v>0.05028767123287672</v>
+      </c>
+      <c r="C9">
+        <v>0.03169590001652978</v>
+      </c>
+      <c r="D9">
+        <v>2061400</v>
+      </c>
+      <c r="E9">
+        <v>262.448652372086</v>
+      </c>
+      <c r="F9">
+        <v>0.01594418699697362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2">
+        <v>30498</v>
+      </c>
+      <c r="B10">
+        <v>0.05038356164383563</v>
+      </c>
+      <c r="C10">
+        <v>0.01593344872708258</v>
+      </c>
+      <c r="D10">
+        <v>2061400</v>
+      </c>
+      <c r="E10">
+        <v>262.4803482721026</v>
+      </c>
+      <c r="F10">
+        <v>0.01608682900022278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>30505</v>
+      </c>
+      <c r="B11">
+        <v>0.05047945205479454</v>
+      </c>
+      <c r="C11">
+        <v>0.01150208359695171</v>
+      </c>
+      <c r="D11">
+        <v>2061400</v>
+      </c>
+      <c r="E11">
+        <v>262.4962817208296</v>
+      </c>
+      <c r="F11">
+        <v>0.01615853477427912</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>30512</v>
+      </c>
+      <c r="B12">
+        <v>0.05057534246575345</v>
+      </c>
+      <c r="C12">
+        <v>0.01091964774695953</v>
+      </c>
+      <c r="D12">
+        <v>2061400</v>
+      </c>
+      <c r="E12">
+        <v>262.5077838044266</v>
+      </c>
+      <c r="F12">
+        <v>0.01621029794380438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>30519</v>
+      </c>
+      <c r="B13">
+        <v>0.05067123287671235</v>
+      </c>
+      <c r="C13">
+        <v>0.01296659871127304</v>
+      </c>
+      <c r="D13">
+        <v>2061400</v>
+      </c>
+      <c r="E13">
+        <v>262.5187034521736</v>
+      </c>
+      <c r="F13">
+        <v>0.01625943995991954</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>30526</v>
+      </c>
+      <c r="B14">
+        <v>0.05076712328767126</v>
+      </c>
+      <c r="C14">
+        <v>0.01230564148090707</v>
+      </c>
+      <c r="D14">
+        <v>2061400</v>
+      </c>
+      <c r="E14">
+        <v>262.5316700508848</v>
+      </c>
+      <c r="F14">
+        <v>0.01631779393045008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2">
+        <v>30533</v>
+      </c>
+      <c r="B15">
+        <v>0.05086301369863017</v>
+      </c>
+      <c r="C15">
+        <v>0.01239144172700435</v>
+      </c>
+      <c r="D15">
+        <v>2061400</v>
+      </c>
+      <c r="E15">
+        <v>262.5439756923657</v>
+      </c>
+      <c r="F15">
+        <v>0.01637317337546323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2">
+        <v>30540</v>
+      </c>
+      <c r="B16">
+        <v>0.05095890410958907</v>
+      </c>
+      <c r="C16">
+        <v>0.0139275113099302</v>
+      </c>
+      <c r="D16">
+        <v>2061400</v>
+      </c>
+      <c r="E16">
+        <v>262.5563671340927</v>
+      </c>
+      <c r="F16">
+        <v>0.01642893894988007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2">
+        <v>30547</v>
+      </c>
+      <c r="B17">
+        <v>0.05105479452054798</v>
+      </c>
+      <c r="C17">
+        <v>0.01278564497260959</v>
+      </c>
+      <c r="D17">
+        <v>2061400</v>
+      </c>
+      <c r="E17">
+        <v>262.5702946454027</v>
+      </c>
+      <c r="F17">
+        <v>0.0164916173440096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>30554</v>
+      </c>
+      <c r="B18">
+        <v>0.05115068493150689</v>
+      </c>
+      <c r="C18">
+        <v>0.01364005245795852</v>
+      </c>
+      <c r="D18">
+        <v>2061400</v>
+      </c>
+      <c r="E18">
+        <v>262.5830802903753</v>
+      </c>
+      <c r="F18">
+        <v>0.01654915696303825</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2">
+        <v>30561</v>
+      </c>
+      <c r="B19">
+        <v>0.05124657534246579</v>
+      </c>
+      <c r="C19">
+        <v>0.01323538896258469</v>
+      </c>
+      <c r="D19">
+        <v>2061400</v>
+      </c>
+      <c r="E19">
+        <v>262.5967203428332</v>
+      </c>
+      <c r="F19">
+        <v>0.01661054169753112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2">
+        <v>30568</v>
+      </c>
+      <c r="B20">
+        <v>0.0513424657534247</v>
+      </c>
+      <c r="C20">
+        <v>0.01364734072581086</v>
+      </c>
+      <c r="D20">
+        <v>2061400</v>
+      </c>
+      <c r="E20">
+        <v>262.6099557317958</v>
+      </c>
+      <c r="F20">
+        <v>0.01667010531283856</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2">
+        <v>30575</v>
+      </c>
+      <c r="B21">
+        <v>0.05143835616438361</v>
+      </c>
+      <c r="C21">
+        <v>0.01274501966418029</v>
+      </c>
+      <c r="D21">
+        <v>2061400</v>
+      </c>
+      <c r="E21">
+        <v>262.6236030725216</v>
+      </c>
+      <c r="F21">
+        <v>0.01673152284694026</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2">
+        <v>30582</v>
+      </c>
+      <c r="B22">
+        <v>0.05153424657534252</v>
+      </c>
+      <c r="C22">
+        <v>0.0124761112537044</v>
+      </c>
+      <c r="D22">
+        <v>2061400</v>
+      </c>
+      <c r="E22">
+        <v>262.6363480921858</v>
+      </c>
+      <c r="F22">
+        <v>0.01678887963868313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2">
+        <v>30589</v>
+      </c>
+      <c r="B23">
+        <v>0.05163013698630142</v>
+      </c>
+      <c r="C23">
+        <v>0.01427151121436054</v>
+      </c>
+      <c r="D23">
+        <v>2061400</v>
+      </c>
+      <c r="E23">
+        <v>262.6488242034395</v>
+      </c>
+      <c r="F23">
+        <v>0.01684502625389384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2">
+        <v>30596</v>
+      </c>
+      <c r="B24">
+        <v>0.05172602739726033</v>
+      </c>
+      <c r="C24">
+        <v>0.01313791919847063</v>
+      </c>
+      <c r="D24">
+        <v>2061400</v>
+      </c>
+      <c r="E24">
+        <v>262.6630957146539</v>
+      </c>
+      <c r="F24">
+        <v>0.01690925276104295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2">
+        <v>30603</v>
+      </c>
+      <c r="B25">
+        <v>0.05182191780821924</v>
+      </c>
+      <c r="C25">
+        <v>0.01342273369471059</v>
+      </c>
+      <c r="D25">
+        <v>2061400</v>
+      </c>
+      <c r="E25">
+        <v>262.6762336338523</v>
+      </c>
+      <c r="F25">
+        <v>0.01696837773026678</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2">
+        <v>30610</v>
+      </c>
+      <c r="B26">
+        <v>0.05191780821917814</v>
+      </c>
+      <c r="C26">
+        <v>0.01433513209792636</v>
+      </c>
+      <c r="D26">
+        <v>2061400</v>
+      </c>
+      <c r="E26">
+        <v>262.6896563675471</v>
+      </c>
+      <c r="F26">
+        <v>0.01702878445865402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2">
+        <v>30617</v>
+      </c>
+      <c r="B27">
+        <v>0.05201369863013705</v>
+      </c>
+      <c r="C27">
+        <v>0.01386727199496818</v>
+      </c>
+      <c r="D27">
+        <v>2061400</v>
+      </c>
+      <c r="E27">
+        <v>262.703991499645</v>
+      </c>
+      <c r="F27">
+        <v>0.01709329728076115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2">
+        <v>30624</v>
+      </c>
+      <c r="B28">
+        <v>0.05210958904109596</v>
+      </c>
+      <c r="C28">
+        <v>0.01344615223217716</v>
+      </c>
+      <c r="D28">
+        <v>2061400</v>
+      </c>
+      <c r="E28">
+        <v>262.71785877164</v>
+      </c>
+      <c r="F28">
+        <v>0.01715570457810667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2">
+        <v>30631</v>
+      </c>
+      <c r="B29">
+        <v>0.05220547945205486</v>
+      </c>
+      <c r="C29">
+        <v>0.01488886179299698</v>
+      </c>
+      <c r="D29">
+        <v>2061400</v>
+      </c>
+      <c r="E29">
+        <v>262.7313049238721</v>
+      </c>
+      <c r="F29">
+        <v>0.01721621669763598</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2">
+        <v>30638</v>
+      </c>
+      <c r="B30">
+        <v>0.05230136986301377</v>
+      </c>
+      <c r="C30">
+        <v>0.01376412211482148</v>
+      </c>
+      <c r="D30">
+        <v>2061400</v>
+      </c>
+      <c r="E30">
+        <v>262.7461937856651</v>
+      </c>
+      <c r="F30">
+        <v>0.01728322148598859</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2">
+        <v>30645</v>
+      </c>
+      <c r="B31">
+        <v>0.05239726027397268</v>
+      </c>
+      <c r="C31">
+        <v>0.01391545029173358</v>
+      </c>
+      <c r="D31">
+        <v>2061400</v>
+      </c>
+      <c r="E31">
+        <v>262.7599579077799</v>
+      </c>
+      <c r="F31">
+        <v>0.01734516457485483</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2">
+        <v>30652</v>
+      </c>
+      <c r="B32">
+        <v>0.05249315068493159</v>
+      </c>
+      <c r="C32">
+        <v>0.01364077628841187</v>
+      </c>
+      <c r="D32">
+        <v>2061400</v>
+      </c>
+      <c r="E32">
+        <v>262.7738733580717</v>
+      </c>
+      <c r="F32">
+        <v>0.01740778869042485</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2">
+        <v>30659</v>
+      </c>
+      <c r="B33">
+        <v>0.05258904109589049</v>
+      </c>
+      <c r="C33">
+        <v>0.01551389475287124</v>
+      </c>
+      <c r="D33">
+        <v>2061400</v>
+      </c>
+      <c r="E33">
+        <v>262.7875141343601</v>
+      </c>
+      <c r="F33">
+        <v>0.01746917668239342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2">
+        <v>30666</v>
+      </c>
+      <c r="B34">
+        <v>0.0526849315068494</v>
+      </c>
+      <c r="C34">
+        <v>0.01413923138170503</v>
+      </c>
+      <c r="D34">
+        <v>2061400</v>
+      </c>
+      <c r="E34">
+        <v>262.803028029113</v>
+      </c>
+      <c r="F34">
+        <v>0.01753899432519856</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2">
+        <v>30673</v>
+      </c>
+      <c r="B35">
+        <v>0.05278082191780831</v>
+      </c>
+      <c r="C35">
+        <v>0.0142525578629602</v>
+      </c>
+      <c r="D35">
+        <v>2061400</v>
+      </c>
+      <c r="E35">
+        <v>262.8171672604947</v>
+      </c>
+      <c r="F35">
+        <v>0.01760262552947541</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2">
+        <v>30680</v>
+      </c>
+      <c r="B36">
+        <v>0.05287671232876721</v>
+      </c>
+      <c r="C36">
+        <v>0.01400891625007716</v>
+      </c>
+      <c r="D36">
+        <v>2061400</v>
+      </c>
+      <c r="E36">
+        <v>262.8314198183576</v>
+      </c>
+      <c r="F36">
+        <v>0.01766676674029256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2">
+        <v>30687</v>
+      </c>
+      <c r="B37">
+        <v>0.05297260273972612</v>
+      </c>
+      <c r="C37">
+        <v>0.01553232033074892</v>
+      </c>
+      <c r="D37">
+        <v>2061400</v>
+      </c>
+      <c r="E37">
+        <v>262.8454287346077</v>
+      </c>
+      <c r="F37">
+        <v>0.0177298114834997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2">
+        <v>30694</v>
+      </c>
+      <c r="B38">
+        <v>0.05306849315068503</v>
+      </c>
+      <c r="C38">
+        <v>0.01441027858959387</v>
+      </c>
+      <c r="D38">
+        <v>2061400</v>
+      </c>
+      <c r="E38">
+        <v>262.8609610549385</v>
+      </c>
+      <c r="F38">
+        <v>0.01779971204748199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>30701</v>
+      </c>
+      <c r="B39">
+        <v>0.05316438356164394</v>
+      </c>
+      <c r="C39">
+        <v>0.0145422738430625</v>
+      </c>
+      <c r="D39">
+        <v>2061400</v>
+      </c>
+      <c r="E39">
+        <v>262.8753713335281</v>
+      </c>
+      <c r="F39">
+        <v>0.01786456305358462</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2">
+        <v>30708</v>
+      </c>
+      <c r="B40">
+        <v>0.05326027397260284</v>
+      </c>
+      <c r="C40">
+        <v>0.01427650402183644</v>
+      </c>
+      <c r="D40">
+        <v>2061400</v>
+      </c>
+      <c r="E40">
+        <v>262.8899136073711</v>
+      </c>
+      <c r="F40">
+        <v>0.01793000808185929</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="2">
+        <v>30715</v>
+      </c>
+      <c r="B41">
+        <v>0.05335616438356175</v>
+      </c>
+      <c r="C41">
+        <v>0.01569610638534868</v>
+      </c>
+      <c r="D41">
+        <v>2061400</v>
+      </c>
+      <c r="E41">
+        <v>262.9041901113929</v>
+      </c>
+      <c r="F41">
+        <v>0.01799425705828866</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="2">
+        <v>30722</v>
+      </c>
+      <c r="B42">
+        <v>0.05345205479452066</v>
+      </c>
+      <c r="C42">
+        <v>0.01459821352341351</v>
+      </c>
+      <c r="D42">
+        <v>2061400</v>
+      </c>
+      <c r="E42">
+        <v>262.9198862177783</v>
+      </c>
+      <c r="F42">
+        <v>0.01806489471353261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="2">
+        <v>30729</v>
+      </c>
+      <c r="B43">
+        <v>0.05354794520547956</v>
+      </c>
+      <c r="C43">
+        <v>0.01475117370569023</v>
+      </c>
+      <c r="D43">
+        <v>2061400</v>
+      </c>
+      <c r="E43">
+        <v>262.9344844313017</v>
+      </c>
+      <c r="F43">
+        <v>0.01813059148881744</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2">
+        <v>30736</v>
+      </c>
+      <c r="B44">
+        <v>0.05364383561643847</v>
+      </c>
+      <c r="C44">
+        <v>0.01447922536272017</v>
+      </c>
+      <c r="D44">
+        <v>2061400</v>
+      </c>
+      <c r="E44">
+        <v>262.9492356050074</v>
+      </c>
+      <c r="F44">
+        <v>0.01819697663536827</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="2">
+        <v>30743</v>
+      </c>
+      <c r="B45">
+        <v>0.05373972602739738</v>
+      </c>
+      <c r="C45">
+        <v>0.01478233413808994</v>
+      </c>
+      <c r="D45">
+        <v>2061400</v>
+      </c>
+      <c r="E45">
+        <v>262.9637148303701</v>
+      </c>
+      <c r="F45">
+        <v>0.01826213792468816</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="2">
+        <v>30750</v>
+      </c>
+      <c r="B46">
+        <v>0.05383561643835628</v>
+      </c>
+      <c r="C46">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>2061400</v>
-      </c>
-      <c r="E2">
-        <v>261.6063956874585</v>
-      </c>
-      <c r="F2">
-        <v>0.01215375414343174</v>
+      <c r="D46">
+        <v>2061400</v>
+      </c>
+      <c r="E46">
+        <v>262.9784971645082</v>
+      </c>
+      <c r="F46">
+        <v>0.01832866330346142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not synching with workspace
</commit_message>
<xml_diff>
--- a/FACModel/Modelled RIHT2.xlsx
+++ b/FACModel/Modelled RIHT2.xlsx
@@ -43,9 +43,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -98,12 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -400,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,26 +424,6 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2">
-        <v>30414</v>
-      </c>
-      <c r="B2">
-        <v>0.03509589041095891</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>2061400</v>
-      </c>
-      <c r="E2">
-        <v>261.6049158331831</v>
-      </c>
-      <c r="F2">
-        <v>0.01214709431114265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>